<commit_message>
sample weather webservice client code
</commit_message>
<xml_diff>
--- a/jee_latest_st.xlsx
+++ b/jee_latest_st.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3437" uniqueCount="1672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3517" uniqueCount="1718">
   <si>
     <t>java server - tomcat</t>
   </si>
@@ -5642,7 +5642,145 @@
     <t>ALL or NOTHING</t>
   </si>
   <si>
-    <t xml:space="preserve"> AA Dotnet program</t>
+    <t>SOAP UI software</t>
+  </si>
+  <si>
+    <t>Soap webservice client (Consuming)</t>
+  </si>
+  <si>
+    <t>&lt;calRect&gt; &lt;num1&gt;20&lt;/num1&gt; &lt;num2&gt;30&lt;/num2&gt;&lt;/calRect&gt;</t>
+  </si>
+  <si>
+    <t>Soap Webservice</t>
+  </si>
+  <si>
+    <t>(publish)</t>
+  </si>
+  <si>
+    <t>public class Math</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>public int add(int a,int b)</t>
+  </si>
+  <si>
+    <t>return a+b;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>&lt;calculateRectangleResponse&gt;&lt;return&gt;600&lt;/return&gt;&lt;/calculateRectangleResponse&gt;</t>
+  </si>
+  <si>
+    <t>Java client</t>
+  </si>
+  <si>
+    <t>STUB program</t>
+  </si>
+  <si>
+    <t>&lt;num1&gt;20&lt;/num1&gt; &lt;num2&gt;30&lt;/num2&gt;</t>
+  </si>
+  <si>
+    <t>Math m=new Math();</t>
+  </si>
+  <si>
+    <t>int result=m.add(10,20);</t>
+  </si>
+  <si>
+    <t>convert client java variables into</t>
+  </si>
+  <si>
+    <t>XML… then make http call to</t>
+  </si>
+  <si>
+    <t>actual webservice</t>
+  </si>
+  <si>
+    <t>&lt;return&gt;600&lt;/return&gt;</t>
+  </si>
+  <si>
+    <t>complex soap response</t>
+  </si>
+  <si>
+    <t>cliennt</t>
+  </si>
+  <si>
+    <t>webservice client</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AA java program</t>
+  </si>
+  <si>
+    <t>HTTP URL</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;soap:calculateRectangle&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;arg0&gt;20&lt;/arg0&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;arg1&gt;10&lt;/arg1&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/soap:calculateRectangle&gt;</t>
+  </si>
+  <si>
+    <t>&lt;soapenv:Envelope/"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;ns2:calculateRectangleResponse xmlns:ns2="http://soap.webservice.tutorial.com/"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         &lt;return&gt;200&lt;/return&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      &lt;/ns2:calculateRectangleResponse&gt;</t>
+  </si>
+  <si>
+    <t>m.add(10,20)</t>
+  </si>
+  <si>
+    <t>========</t>
+  </si>
+  <si>
+    <t>STUB program converts our method input into complex soap request</t>
+  </si>
+  <si>
+    <t>=========</t>
+  </si>
+  <si>
+    <t>int result</t>
+  </si>
+  <si>
+    <t>STUB Program convert complex soap response into simple java variable</t>
+  </si>
+  <si>
+    <t>weather.html</t>
+  </si>
+  <si>
+    <t>WeatherServlet</t>
+  </si>
+  <si>
+    <t>Newyork</t>
+  </si>
+  <si>
+    <t>openweather.com</t>
+  </si>
+  <si>
+    <t>Rest Weather webservice</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
   </si>
 </sst>
 </file>
@@ -6421,7 +6559,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="575">
+  <cellXfs count="581">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -7238,18 +7376,6 @@
     <xf numFmtId="0" fontId="0" fillId="22" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -7271,8 +7397,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -7304,9 +7445,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7316,8 +7454,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7373,57 +7562,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7445,53 +7583,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7532,21 +7634,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -17997,10 +18141,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:Q203"/>
+  <dimension ref="A2:Q261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:J31"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I256" sqref="I256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18035,7 +18179,7 @@
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1">
       <c r="D6" s="4"/>
-      <c r="E6" s="472" t="s">
+      <c r="E6" s="479" t="s">
         <v>406</v>
       </c>
       <c r="F6" s="417"/>
@@ -18056,7 +18200,7 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="2:17" ht="15" customHeight="1">
-      <c r="D7" s="480">
+      <c r="D7" s="476">
         <v>80</v>
       </c>
       <c r="E7" s="147"/>
@@ -18074,7 +18218,7 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="2:17" ht="15" customHeight="1">
-      <c r="D8" s="480"/>
+      <c r="D8" s="476"/>
       <c r="E8" s="134" t="s">
         <v>408</v>
       </c>
@@ -18109,7 +18253,7 @@
       <c r="B9" t="s">
         <v>407</v>
       </c>
-      <c r="D9" s="480"/>
+      <c r="D9" s="476"/>
       <c r="E9" s="149"/>
       <c r="F9" s="344"/>
       <c r="G9" s="149"/>
@@ -18133,7 +18277,7 @@
       <c r="Q9" s="6"/>
     </row>
     <row r="10" spans="2:17" ht="15" customHeight="1">
-      <c r="D10" s="480"/>
+      <c r="D10" s="476"/>
       <c r="E10" s="147"/>
       <c r="F10" s="148"/>
       <c r="G10" s="147"/>
@@ -18157,7 +18301,7 @@
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="2:17" ht="15" customHeight="1">
-      <c r="D11" s="480"/>
+      <c r="D11" s="476"/>
       <c r="E11" s="134" t="s">
         <v>412</v>
       </c>
@@ -18186,7 +18330,7 @@
       <c r="B12" s="209" t="s">
         <v>416</v>
       </c>
-      <c r="D12" s="480"/>
+      <c r="D12" s="476"/>
       <c r="E12" s="149"/>
       <c r="F12" s="344"/>
       <c r="G12" s="149"/>
@@ -18204,7 +18348,7 @@
       <c r="Q12" s="6"/>
     </row>
     <row r="13" spans="2:17" ht="15" customHeight="1">
-      <c r="D13" s="480"/>
+      <c r="D13" s="476"/>
       <c r="E13" s="147"/>
       <c r="F13" s="148"/>
       <c r="G13" s="147"/>
@@ -18220,7 +18364,7 @@
       <c r="Q13" s="6"/>
     </row>
     <row r="14" spans="2:17" ht="15" customHeight="1">
-      <c r="D14" s="480"/>
+      <c r="D14" s="476"/>
       <c r="E14" s="134" t="s">
         <v>417</v>
       </c>
@@ -18244,7 +18388,7 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="2:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D15" s="480"/>
+      <c r="D15" s="476"/>
       <c r="E15" s="149"/>
       <c r="F15" s="344"/>
       <c r="G15" s="149"/>
@@ -18260,7 +18404,7 @@
       <c r="Q15" s="6"/>
     </row>
     <row r="16" spans="2:17" ht="15" customHeight="1">
-      <c r="D16" s="480"/>
+      <c r="D16" s="476"/>
       <c r="E16" s="147"/>
       <c r="F16" s="148"/>
       <c r="G16" s="24"/>
@@ -18276,7 +18420,7 @@
       <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="1:17" ht="15" customHeight="1">
-      <c r="D17" s="480"/>
+      <c r="D17" s="476"/>
       <c r="E17" s="134" t="s">
         <v>421</v>
       </c>
@@ -18300,7 +18444,7 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" thickBot="1">
-      <c r="D18" s="480"/>
+      <c r="D18" s="476"/>
       <c r="E18" s="149"/>
       <c r="F18" s="344"/>
       <c r="G18" s="71"/>
@@ -18317,20 +18461,20 @@
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1">
       <c r="D19" s="8"/>
-      <c r="E19" s="473" t="s">
+      <c r="E19" s="480" t="s">
         <v>194</v>
       </c>
-      <c r="F19" s="474"/>
-      <c r="G19" s="473" t="s">
+      <c r="F19" s="481"/>
+      <c r="G19" s="480" t="s">
         <v>195</v>
       </c>
-      <c r="H19" s="474"/>
-      <c r="I19" s="473" t="s">
+      <c r="H19" s="481"/>
+      <c r="I19" s="480" t="s">
         <v>196</v>
       </c>
-      <c r="J19" s="475"/>
-      <c r="K19" s="475"/>
-      <c r="L19" s="474"/>
+      <c r="J19" s="482"/>
+      <c r="K19" s="482"/>
+      <c r="L19" s="481"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -18395,12 +18539,12 @@
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="482"/>
-      <c r="H24" s="482"/>
-      <c r="I24" s="482"/>
-      <c r="J24" s="482"/>
-      <c r="K24" s="482"/>
-      <c r="L24" s="482"/>
+      <c r="G24" s="478"/>
+      <c r="H24" s="478"/>
+      <c r="I24" s="478"/>
+      <c r="J24" s="478"/>
+      <c r="K24" s="478"/>
+      <c r="L24" s="478"/>
       <c r="O24" s="40" t="s">
         <v>179</v>
       </c>
@@ -18716,7 +18860,9 @@
         <v>547</v>
       </c>
       <c r="G44" s="4"/>
-      <c r="H44" s="5"/>
+      <c r="H44" s="288" t="s">
+        <v>1693</v>
+      </c>
       <c r="I44" s="5"/>
       <c r="J44" s="6"/>
       <c r="L44" t="s">
@@ -18745,6 +18891,9 @@
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="1:17">
+      <c r="A46" s="575" t="s">
+        <v>429</v>
+      </c>
       <c r="C46" s="4"/>
       <c r="D46" s="6" t="s">
         <v>442</v>
@@ -18768,6 +18917,9 @@
       </c>
     </row>
     <row r="47" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A47" s="575" t="s">
+        <v>1692</v>
+      </c>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="G47" s="222" t="s">
@@ -18776,7 +18928,7 @@
       <c r="H47" s="468" t="s">
         <v>1353</v>
       </c>
-      <c r="I47" s="481"/>
+      <c r="I47" s="477"/>
       <c r="J47" s="469"/>
     </row>
     <row r="48" spans="1:17">
@@ -18885,7 +19037,7 @@
       <c r="G53" s="20" t="s">
         <v>846</v>
       </c>
-      <c r="H53" s="218" t="s">
+      <c r="H53" s="576" t="s">
         <v>851</v>
       </c>
       <c r="J53" s="35" t="s">
@@ -18910,7 +19062,7 @@
         <v>427</v>
       </c>
       <c r="G54" s="220" t="s">
-        <v>1671</v>
+        <v>1694</v>
       </c>
       <c r="H54" s="219"/>
       <c r="I54" t="s">
@@ -19383,16 +19535,16 @@
         <v>1047</v>
       </c>
       <c r="F131" s="38"/>
-      <c r="G131" s="478" t="s">
+      <c r="G131" s="474" t="s">
         <v>1040</v>
       </c>
-      <c r="H131" s="478"/>
-      <c r="I131" s="478"/>
-      <c r="J131" s="478"/>
-      <c r="K131" s="478"/>
-      <c r="L131" s="478"/>
-      <c r="M131" s="478"/>
-      <c r="N131" s="478"/>
+      <c r="H131" s="474"/>
+      <c r="I131" s="474"/>
+      <c r="J131" s="474"/>
+      <c r="K131" s="474"/>
+      <c r="L131" s="474"/>
+      <c r="M131" s="474"/>
+      <c r="N131" s="474"/>
       <c r="O131" s="38"/>
     </row>
     <row r="132" spans="2:15">
@@ -19529,29 +19681,29 @@
     </row>
     <row r="141" spans="2:15">
       <c r="F141" s="38"/>
-      <c r="G141" s="479"/>
-      <c r="H141" s="479"/>
-      <c r="I141" s="479"/>
-      <c r="J141" s="479"/>
-      <c r="K141" s="479"/>
-      <c r="L141" s="479"/>
-      <c r="M141" s="479"/>
-      <c r="N141" s="479"/>
-      <c r="O141" s="479"/>
+      <c r="G141" s="475"/>
+      <c r="H141" s="475"/>
+      <c r="I141" s="475"/>
+      <c r="J141" s="475"/>
+      <c r="K141" s="475"/>
+      <c r="L141" s="475"/>
+      <c r="M141" s="475"/>
+      <c r="N141" s="475"/>
+      <c r="O141" s="475"/>
     </row>
     <row r="142" spans="2:15">
       <c r="F142" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G142" s="479"/>
-      <c r="H142" s="479"/>
-      <c r="I142" s="479"/>
-      <c r="J142" s="479"/>
-      <c r="K142" s="479"/>
-      <c r="L142" s="479"/>
-      <c r="M142" s="479"/>
-      <c r="N142" s="479"/>
-      <c r="O142" s="479"/>
+      <c r="G142" s="475"/>
+      <c r="H142" s="475"/>
+      <c r="I142" s="475"/>
+      <c r="J142" s="475"/>
+      <c r="K142" s="475"/>
+      <c r="L142" s="475"/>
+      <c r="M142" s="475"/>
+      <c r="N142" s="475"/>
+      <c r="O142" s="475"/>
     </row>
     <row r="146" spans="4:13">
       <c r="F146" t="s">
@@ -19595,7 +19747,7 @@
     </row>
     <row r="157" spans="4:13" ht="15.75" thickBot="1"/>
     <row r="158" spans="4:13">
-      <c r="D158" s="476" t="s">
+      <c r="D158" s="472" t="s">
         <v>1319</v>
       </c>
       <c r="E158" s="66"/>
@@ -19608,7 +19760,7 @@
       <c r="L158" s="237"/>
     </row>
     <row r="159" spans="4:13">
-      <c r="D159" s="477"/>
+      <c r="D159" s="473"/>
       <c r="E159" s="313" t="s">
         <v>1317</v>
       </c>
@@ -19630,7 +19782,7 @@
       </c>
     </row>
     <row r="160" spans="4:13" ht="15.75" thickBot="1">
-      <c r="D160" s="477"/>
+      <c r="D160" s="473"/>
       <c r="E160" s="232"/>
       <c r="F160" s="238"/>
       <c r="G160" s="232"/>
@@ -19641,7 +19793,7 @@
       <c r="L160" s="238"/>
     </row>
     <row r="161" spans="4:13">
-      <c r="D161" s="477"/>
+      <c r="D161" s="473"/>
       <c r="E161" s="315"/>
       <c r="F161" s="316"/>
       <c r="G161" s="315"/>
@@ -19652,7 +19804,7 @@
       <c r="L161" s="316"/>
     </row>
     <row r="162" spans="4:13">
-      <c r="D162" s="477"/>
+      <c r="D162" s="473"/>
       <c r="E162" s="317"/>
       <c r="F162" s="318"/>
       <c r="G162" s="317"/>
@@ -19666,7 +19818,7 @@
       </c>
     </row>
     <row r="163" spans="4:13" ht="15.75" thickBot="1">
-      <c r="D163" s="477"/>
+      <c r="D163" s="473"/>
       <c r="E163" s="319"/>
       <c r="F163" s="320"/>
       <c r="G163" s="319"/>
@@ -19677,7 +19829,7 @@
       <c r="L163" s="320"/>
     </row>
     <row r="164" spans="4:13">
-      <c r="D164" s="477"/>
+      <c r="D164" s="473"/>
       <c r="E164" s="66"/>
       <c r="F164" s="237"/>
       <c r="G164" s="66"/>
@@ -19688,7 +19840,7 @@
       <c r="L164" s="237"/>
     </row>
     <row r="165" spans="4:13">
-      <c r="D165" s="477"/>
+      <c r="D165" s="473"/>
       <c r="E165" s="58"/>
       <c r="F165" s="312"/>
       <c r="G165" s="58"/>
@@ -19702,7 +19854,7 @@
       </c>
     </row>
     <row r="166" spans="4:13" ht="15.75" thickBot="1">
-      <c r="D166" s="477"/>
+      <c r="D166" s="473"/>
       <c r="E166" s="232"/>
       <c r="F166" s="238"/>
       <c r="G166" s="232"/>
@@ -19713,7 +19865,7 @@
       <c r="L166" s="238"/>
     </row>
     <row r="167" spans="4:13">
-      <c r="D167" s="477"/>
+      <c r="D167" s="473"/>
       <c r="E167" s="66"/>
       <c r="F167" s="237"/>
       <c r="G167" s="59"/>
@@ -19724,7 +19876,7 @@
       <c r="L167" s="312"/>
     </row>
     <row r="168" spans="4:13">
-      <c r="D168" s="477"/>
+      <c r="D168" s="473"/>
       <c r="E168" s="58"/>
       <c r="F168" s="312"/>
       <c r="G168" s="59"/>
@@ -19738,7 +19890,7 @@
       </c>
     </row>
     <row r="169" spans="4:13" ht="15.75" thickBot="1">
-      <c r="D169" s="477"/>
+      <c r="D169" s="473"/>
       <c r="E169" s="232"/>
       <c r="F169" s="238"/>
       <c r="G169" s="321"/>
@@ -19916,19 +20068,586 @@
       <c r="J203" s="40"/>
       <c r="L203" s="40"/>
     </row>
+    <row r="209" spans="1:14">
+      <c r="D209" t="s">
+        <v>1696</v>
+      </c>
+      <c r="F209" t="s">
+        <v>1695</v>
+      </c>
+      <c r="G209" t="s">
+        <v>1697</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14">
+      <c r="A210" t="s">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A211" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E211" t="s">
+        <v>1673</v>
+      </c>
+      <c r="L211" t="s">
+        <v>1674</v>
+      </c>
+      <c r="N211" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14">
+      <c r="A212" s="1"/>
+      <c r="B212" s="2"/>
+      <c r="C212" s="3"/>
+      <c r="H212" t="s">
+        <v>431</v>
+      </c>
+      <c r="L212" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="M212" s="2"/>
+      <c r="N212" s="3"/>
+    </row>
+    <row r="213" spans="1:14">
+      <c r="A213" s="4"/>
+      <c r="B213" s="5"/>
+      <c r="C213" s="6"/>
+      <c r="D213" t="s">
+        <v>1677</v>
+      </c>
+      <c r="L213" s="4" t="s">
+        <v>1678</v>
+      </c>
+      <c r="M213" s="5"/>
+      <c r="N213" s="6"/>
+    </row>
+    <row r="214" spans="1:14">
+      <c r="A214" s="4"/>
+      <c r="B214" s="5"/>
+      <c r="C214" s="6"/>
+      <c r="L214" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="M214" s="5"/>
+      <c r="N214" s="6"/>
+    </row>
+    <row r="215" spans="1:14">
+      <c r="A215" s="4"/>
+      <c r="B215" s="5"/>
+      <c r="C215" s="6"/>
+      <c r="H215" t="s">
+        <v>431</v>
+      </c>
+      <c r="L215" s="4"/>
+      <c r="M215" s="5" t="s">
+        <v>1679</v>
+      </c>
+      <c r="N215" s="6"/>
+    </row>
+    <row r="216" spans="1:14">
+      <c r="A216" s="4"/>
+      <c r="B216" s="5"/>
+      <c r="C216" s="6"/>
+      <c r="D216" t="s">
+        <v>1680</v>
+      </c>
+      <c r="L216" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="M216" s="5"/>
+      <c r="N216" s="6"/>
+    </row>
+    <row r="217" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A217" s="8"/>
+      <c r="B217" s="10"/>
+      <c r="C217" s="9"/>
+      <c r="E217" t="s">
+        <v>1681</v>
+      </c>
+      <c r="L217" s="8"/>
+      <c r="M217" s="10"/>
+      <c r="N217" s="9"/>
+    </row>
+    <row r="220" spans="1:14">
+      <c r="A220" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="221" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A221" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E221" t="s">
+        <v>1683</v>
+      </c>
+      <c r="H221" t="s">
+        <v>1684</v>
+      </c>
+      <c r="L221" t="s">
+        <v>1674</v>
+      </c>
+      <c r="N221" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="222" spans="1:14">
+      <c r="A222" s="1"/>
+      <c r="B222" s="2"/>
+      <c r="C222" s="3"/>
+      <c r="E222" s="248" t="s">
+        <v>1676</v>
+      </c>
+      <c r="F222" s="56"/>
+      <c r="G222" s="57"/>
+      <c r="I222" t="s">
+        <v>431</v>
+      </c>
+      <c r="L222" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="M222" s="2"/>
+      <c r="N222" s="3"/>
+    </row>
+    <row r="223" spans="1:14">
+      <c r="A223" s="4" t="s">
+        <v>1685</v>
+      </c>
+      <c r="B223" s="5"/>
+      <c r="C223" s="6"/>
+      <c r="D223" t="s">
+        <v>1677</v>
+      </c>
+      <c r="E223" s="35" t="s">
+        <v>1678</v>
+      </c>
+      <c r="F223" s="28"/>
+      <c r="G223" s="39"/>
+      <c r="H223" t="s">
+        <v>485</v>
+      </c>
+      <c r="L223" s="4" t="s">
+        <v>1678</v>
+      </c>
+      <c r="M223" s="5"/>
+      <c r="N223" s="6"/>
+    </row>
+    <row r="224" spans="1:14">
+      <c r="A224" s="4" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B224" s="5"/>
+      <c r="C224" s="6"/>
+      <c r="E224" s="35" t="s">
+        <v>549</v>
+      </c>
+      <c r="F224" s="28"/>
+      <c r="G224" s="39"/>
+      <c r="L224" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="M224" s="5"/>
+      <c r="N224" s="6"/>
+    </row>
+    <row r="225" spans="1:14">
+      <c r="A225" s="4"/>
+      <c r="B225" s="5"/>
+      <c r="C225" s="6"/>
+      <c r="E225" s="577" t="s">
+        <v>1687</v>
+      </c>
+      <c r="F225" s="578"/>
+      <c r="G225" s="579"/>
+      <c r="I225" t="s">
+        <v>431</v>
+      </c>
+      <c r="L225" s="4"/>
+      <c r="M225" s="122" t="s">
+        <v>1679</v>
+      </c>
+      <c r="N225" s="6"/>
+    </row>
+    <row r="226" spans="1:14">
+      <c r="A226" s="4"/>
+      <c r="B226" s="5"/>
+      <c r="C226" s="6"/>
+      <c r="D226" t="s">
+        <v>1680</v>
+      </c>
+      <c r="E226" s="577" t="s">
+        <v>1688</v>
+      </c>
+      <c r="F226" s="578"/>
+      <c r="G226" s="579"/>
+      <c r="H226" t="s">
+        <v>486</v>
+      </c>
+      <c r="L226" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="M226" s="5"/>
+      <c r="N226" s="6"/>
+    </row>
+    <row r="227" spans="1:14">
+      <c r="A227" s="4"/>
+      <c r="B227" s="5"/>
+      <c r="C227" s="6"/>
+      <c r="E227" s="577" t="s">
+        <v>1689</v>
+      </c>
+      <c r="F227" s="578"/>
+      <c r="G227" s="579"/>
+      <c r="I227" t="s">
+        <v>1690</v>
+      </c>
+      <c r="L227" s="4"/>
+      <c r="M227" s="5"/>
+      <c r="N227" s="6"/>
+    </row>
+    <row r="228" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A228" s="8"/>
+      <c r="B228" s="10"/>
+      <c r="C228" s="9"/>
+      <c r="E228" s="249" t="s">
+        <v>236</v>
+      </c>
+      <c r="F228" s="305"/>
+      <c r="G228" s="250"/>
+      <c r="I228" t="s">
+        <v>1691</v>
+      </c>
+      <c r="L228" s="8"/>
+      <c r="M228" s="10"/>
+      <c r="N228" s="9"/>
+    </row>
+    <row r="230" spans="1:14">
+      <c r="A230" s="5" t="s">
+        <v>1706</v>
+      </c>
+      <c r="I230" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="231" spans="1:14">
+      <c r="A231" s="580" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B231" t="s">
+        <v>1708</v>
+      </c>
+      <c r="I231" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="232" spans="1:14">
+      <c r="A232" t="s">
+        <v>1702</v>
+      </c>
+      <c r="I232" t="s">
+        <v>1703</v>
+      </c>
+    </row>
+    <row r="233" spans="1:14">
+      <c r="A233" t="s">
+        <v>497</v>
+      </c>
+      <c r="I233" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="234" spans="1:14">
+      <c r="A234" t="s">
+        <v>498</v>
+      </c>
+      <c r="I234" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="235" spans="1:14">
+      <c r="A235" t="s">
+        <v>1698</v>
+      </c>
+      <c r="I235" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="236" spans="1:14">
+      <c r="A236" t="s">
+        <v>1699</v>
+      </c>
+      <c r="I236" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="237" spans="1:14">
+      <c r="A237" t="s">
+        <v>1700</v>
+      </c>
+      <c r="I237" s="580" t="s">
+        <v>1709</v>
+      </c>
+      <c r="J237" t="s">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="238" spans="1:14">
+      <c r="A238" t="s">
+        <v>1701</v>
+      </c>
+      <c r="I238" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="239" spans="1:14">
+      <c r="A239" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="240" spans="1:14">
+      <c r="A240" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="241" spans="2:14" ht="15.75" thickBot="1"/>
+    <row r="242" spans="2:14">
+      <c r="G242" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H242" s="2"/>
+      <c r="I242" s="2"/>
+      <c r="J242" s="2"/>
+      <c r="K242" s="2"/>
+      <c r="L242" s="2"/>
+      <c r="M242" s="2"/>
+      <c r="N242" s="3"/>
+    </row>
+    <row r="243" spans="2:14" ht="15.75" thickBot="1">
+      <c r="G243" s="4"/>
+      <c r="H243" s="5"/>
+      <c r="I243" s="5"/>
+      <c r="J243" s="5"/>
+      <c r="K243" s="5"/>
+      <c r="L243" s="5"/>
+      <c r="M243" s="5"/>
+      <c r="N243" s="6"/>
+    </row>
+    <row r="244" spans="2:14">
+      <c r="B244" s="1" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C244" s="2"/>
+      <c r="D244" s="3"/>
+      <c r="G244" s="4"/>
+      <c r="H244" s="1"/>
+      <c r="I244" s="2"/>
+      <c r="J244" s="2"/>
+      <c r="K244" s="2"/>
+      <c r="L244" s="2"/>
+      <c r="M244" s="3"/>
+      <c r="N244" s="6"/>
+    </row>
+    <row r="245" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B245" s="4"/>
+      <c r="C245" s="5"/>
+      <c r="D245" s="6"/>
+      <c r="G245" s="4"/>
+      <c r="H245" s="4"/>
+      <c r="I245" s="5"/>
+      <c r="J245" s="5"/>
+      <c r="K245" s="5"/>
+      <c r="L245" s="5"/>
+      <c r="M245" s="6"/>
+      <c r="N245" s="6"/>
+    </row>
+    <row r="246" spans="2:14">
+      <c r="B246" s="4"/>
+      <c r="C246" s="5"/>
+      <c r="D246" s="6"/>
+      <c r="G246" s="4"/>
+      <c r="H246" s="4"/>
+      <c r="I246" s="5"/>
+      <c r="J246" s="1" t="s">
+        <v>1713</v>
+      </c>
+      <c r="K246" s="2"/>
+      <c r="L246" s="3"/>
+      <c r="M246" s="6"/>
+      <c r="N246" s="6"/>
+    </row>
+    <row r="247" spans="2:14">
+      <c r="B247" s="4"/>
+      <c r="C247" s="5" t="s">
+        <v>1714</v>
+      </c>
+      <c r="D247" s="6"/>
+      <c r="E247" t="s">
+        <v>947</v>
+      </c>
+      <c r="G247" s="4"/>
+      <c r="H247" s="4"/>
+      <c r="I247" s="5"/>
+      <c r="J247" s="4"/>
+      <c r="K247" s="5"/>
+      <c r="L247" s="6"/>
+      <c r="M247" s="6"/>
+      <c r="N247" s="6"/>
+    </row>
+    <row r="248" spans="2:14">
+      <c r="B248" s="4"/>
+      <c r="C248" s="5"/>
+      <c r="D248" s="6"/>
+      <c r="G248" s="4"/>
+      <c r="H248" s="4"/>
+      <c r="I248" s="5"/>
+      <c r="J248" s="4"/>
+      <c r="K248" s="5" t="s">
+        <v>1693</v>
+      </c>
+      <c r="L248" s="6"/>
+      <c r="M248" s="6"/>
+      <c r="N248" s="6"/>
+    </row>
+    <row r="249" spans="2:14" ht="15.75" thickBot="1">
+      <c r="B249" s="8"/>
+      <c r="C249" s="10"/>
+      <c r="D249" s="9"/>
+      <c r="E249" t="s">
+        <v>1717</v>
+      </c>
+      <c r="G249" s="4"/>
+      <c r="H249" s="4"/>
+      <c r="I249" s="5"/>
+      <c r="J249" s="8"/>
+      <c r="K249" s="305"/>
+      <c r="L249" s="9"/>
+      <c r="M249" s="6"/>
+      <c r="N249" s="6"/>
+    </row>
+    <row r="250" spans="2:14">
+      <c r="G250" s="4"/>
+      <c r="H250" s="4"/>
+      <c r="I250" s="5"/>
+      <c r="J250" s="5"/>
+      <c r="K250" s="28"/>
+      <c r="L250" s="5"/>
+      <c r="M250" s="6"/>
+      <c r="N250" s="6"/>
+    </row>
+    <row r="251" spans="2:14" ht="15.75" thickBot="1">
+      <c r="G251" s="4"/>
+      <c r="H251" s="8"/>
+      <c r="I251" s="10"/>
+      <c r="J251" s="10"/>
+      <c r="K251" s="305"/>
+      <c r="L251" s="10"/>
+      <c r="M251" s="9"/>
+      <c r="N251" s="6"/>
+    </row>
+    <row r="252" spans="2:14" ht="15.75" thickBot="1">
+      <c r="G252" s="8"/>
+      <c r="H252" s="10"/>
+      <c r="I252" s="10"/>
+      <c r="J252" s="10"/>
+      <c r="K252" s="305"/>
+      <c r="L252" s="10"/>
+      <c r="M252" s="10"/>
+      <c r="N252" s="9"/>
+    </row>
+    <row r="253" spans="2:14">
+      <c r="K253" s="40"/>
+    </row>
+    <row r="254" spans="2:14" ht="15.75" thickBot="1">
+      <c r="K254" s="40"/>
+    </row>
+    <row r="255" spans="2:14">
+      <c r="G255" s="1" t="s">
+        <v>1715</v>
+      </c>
+      <c r="H255" s="2"/>
+      <c r="I255" s="2"/>
+      <c r="J255" s="2"/>
+      <c r="K255" s="56"/>
+      <c r="L255" s="2"/>
+      <c r="M255" s="2"/>
+      <c r="N255" s="3"/>
+    </row>
+    <row r="256" spans="2:14" ht="15.75" thickBot="1">
+      <c r="G256" s="4"/>
+      <c r="H256" s="5"/>
+      <c r="I256" s="5"/>
+      <c r="J256" s="5"/>
+      <c r="K256" s="28"/>
+      <c r="L256" s="5"/>
+      <c r="M256" s="5"/>
+      <c r="N256" s="6"/>
+    </row>
+    <row r="257" spans="7:14">
+      <c r="G257" s="4"/>
+      <c r="H257" s="5"/>
+      <c r="I257" s="5"/>
+      <c r="J257" s="1" t="s">
+        <v>1716</v>
+      </c>
+      <c r="K257" s="2"/>
+      <c r="L257" s="2"/>
+      <c r="M257" s="3"/>
+      <c r="N257" s="6"/>
+    </row>
+    <row r="258" spans="7:14">
+      <c r="G258" s="4"/>
+      <c r="H258" s="5"/>
+      <c r="I258" s="5"/>
+      <c r="J258" s="4"/>
+      <c r="K258" s="5"/>
+      <c r="L258" s="5"/>
+      <c r="M258" s="6"/>
+      <c r="N258" s="6"/>
+    </row>
+    <row r="259" spans="7:14">
+      <c r="G259" s="4"/>
+      <c r="H259" s="5"/>
+      <c r="I259" s="5"/>
+      <c r="J259" s="4"/>
+      <c r="K259" s="5"/>
+      <c r="L259" s="5"/>
+      <c r="M259" s="6"/>
+      <c r="N259" s="6"/>
+    </row>
+    <row r="260" spans="7:14" ht="15.75" thickBot="1">
+      <c r="G260" s="4"/>
+      <c r="H260" s="5"/>
+      <c r="I260" s="5"/>
+      <c r="J260" s="8"/>
+      <c r="K260" s="10"/>
+      <c r="L260" s="10"/>
+      <c r="M260" s="9"/>
+      <c r="N260" s="6"/>
+    </row>
+    <row r="261" spans="7:14" ht="15.75" thickBot="1">
+      <c r="G261" s="8"/>
+      <c r="H261" s="10"/>
+      <c r="I261" s="10"/>
+      <c r="J261" s="10"/>
+      <c r="K261" s="10"/>
+      <c r="L261" s="10"/>
+      <c r="M261" s="10"/>
+      <c r="N261" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:L19"/>
     <mergeCell ref="D158:D169"/>
     <mergeCell ref="G131:N131"/>
     <mergeCell ref="G141:O142"/>
     <mergeCell ref="D7:D18"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="G24:L24"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:L19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P9" r:id="rId1"/>
@@ -20190,7 +20909,7 @@
       <c r="N20" s="38"/>
     </row>
     <row r="21" spans="3:14">
-      <c r="C21" s="494">
+      <c r="C21" s="484">
         <v>43909</v>
       </c>
       <c r="D21" s="483"/>
@@ -20210,7 +20929,7 @@
       <c r="N21" s="483"/>
     </row>
     <row r="22" spans="3:14">
-      <c r="C22" s="494"/>
+      <c r="C22" s="484"/>
       <c r="D22" s="483"/>
       <c r="E22" s="483"/>
       <c r="F22" s="483"/>
@@ -20228,7 +20947,7 @@
       <c r="N22" s="38"/>
     </row>
     <row r="23" spans="3:14">
-      <c r="C23" s="494"/>
+      <c r="C23" s="484"/>
       <c r="D23" s="483"/>
       <c r="E23" s="483"/>
       <c r="F23" s="483"/>
@@ -20244,7 +20963,7 @@
       <c r="N23" s="483"/>
     </row>
     <row r="24" spans="3:14">
-      <c r="C24" s="494"/>
+      <c r="C24" s="484"/>
       <c r="D24" s="483"/>
       <c r="E24" s="483"/>
       <c r="F24" s="483"/>
@@ -20283,16 +21002,16 @@
       <c r="C26" s="116">
         <v>43911</v>
       </c>
-      <c r="D26" s="484"/>
-      <c r="E26" s="485"/>
-      <c r="F26" s="485"/>
-      <c r="G26" s="485"/>
-      <c r="H26" s="486"/>
-      <c r="I26" s="491" t="s">
+      <c r="D26" s="485"/>
+      <c r="E26" s="486"/>
+      <c r="F26" s="486"/>
+      <c r="G26" s="486"/>
+      <c r="H26" s="487"/>
+      <c r="I26" s="492" t="s">
         <v>460</v>
       </c>
-      <c r="J26" s="484"/>
-      <c r="K26" s="486"/>
+      <c r="J26" s="485"/>
+      <c r="K26" s="487"/>
       <c r="L26" s="117" t="s">
         <v>461</v>
       </c>
@@ -20301,14 +21020,14 @@
     </row>
     <row r="27" spans="3:14">
       <c r="C27" s="38"/>
-      <c r="D27" s="487"/>
-      <c r="E27" s="482"/>
-      <c r="F27" s="482"/>
-      <c r="G27" s="482"/>
-      <c r="H27" s="488"/>
-      <c r="I27" s="492"/>
-      <c r="J27" s="487"/>
-      <c r="K27" s="488"/>
+      <c r="D27" s="488"/>
+      <c r="E27" s="478"/>
+      <c r="F27" s="478"/>
+      <c r="G27" s="478"/>
+      <c r="H27" s="489"/>
+      <c r="I27" s="493"/>
+      <c r="J27" s="488"/>
+      <c r="K27" s="489"/>
       <c r="L27" s="483" t="s">
         <v>465</v>
       </c>
@@ -20317,14 +21036,14 @@
     </row>
     <row r="28" spans="3:14">
       <c r="C28" s="38"/>
-      <c r="D28" s="487"/>
-      <c r="E28" s="482"/>
-      <c r="F28" s="482"/>
-      <c r="G28" s="482"/>
-      <c r="H28" s="488"/>
-      <c r="I28" s="492"/>
-      <c r="J28" s="487"/>
-      <c r="K28" s="488"/>
+      <c r="D28" s="488"/>
+      <c r="E28" s="478"/>
+      <c r="F28" s="478"/>
+      <c r="G28" s="478"/>
+      <c r="H28" s="489"/>
+      <c r="I28" s="493"/>
+      <c r="J28" s="488"/>
+      <c r="K28" s="489"/>
       <c r="L28" s="118" t="s">
         <v>460</v>
       </c>
@@ -20333,14 +21052,14 @@
     </row>
     <row r="29" spans="3:14">
       <c r="C29" s="38"/>
-      <c r="D29" s="489"/>
+      <c r="D29" s="490"/>
       <c r="E29" s="470"/>
       <c r="F29" s="470"/>
       <c r="G29" s="470"/>
-      <c r="H29" s="490"/>
-      <c r="I29" s="493"/>
-      <c r="J29" s="489"/>
-      <c r="K29" s="490"/>
+      <c r="H29" s="491"/>
+      <c r="I29" s="494"/>
+      <c r="J29" s="490"/>
+      <c r="K29" s="491"/>
       <c r="L29" s="119" t="s">
         <v>466</v>
       </c>
@@ -20405,7 +21124,7 @@
       <c r="N33" s="38"/>
     </row>
     <row r="34" spans="1:14">
-      <c r="C34" s="494">
+      <c r="C34" s="484">
         <v>43909</v>
       </c>
       <c r="D34" s="483"/>
@@ -20423,7 +21142,7 @@
       <c r="N34" s="483"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="C35" s="494"/>
+      <c r="C35" s="484"/>
       <c r="D35" s="483"/>
       <c r="E35" s="483"/>
       <c r="F35" s="483"/>
@@ -20439,7 +21158,7 @@
       <c r="N35" s="38"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="C36" s="494"/>
+      <c r="C36" s="484"/>
       <c r="D36" s="483"/>
       <c r="E36" s="483"/>
       <c r="F36" s="483"/>
@@ -20455,7 +21174,7 @@
       <c r="N36" s="483"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="C37" s="494"/>
+      <c r="C37" s="484"/>
       <c r="D37" s="483"/>
       <c r="E37" s="483"/>
       <c r="F37" s="483"/>
@@ -20494,14 +21213,14 @@
       <c r="C39" s="116">
         <v>43911</v>
       </c>
-      <c r="D39" s="484"/>
-      <c r="E39" s="485"/>
-      <c r="F39" s="485"/>
-      <c r="G39" s="485"/>
-      <c r="H39" s="486"/>
-      <c r="I39" s="491"/>
-      <c r="J39" s="484"/>
-      <c r="K39" s="486"/>
+      <c r="D39" s="485"/>
+      <c r="E39" s="486"/>
+      <c r="F39" s="486"/>
+      <c r="G39" s="486"/>
+      <c r="H39" s="487"/>
+      <c r="I39" s="492"/>
+      <c r="J39" s="485"/>
+      <c r="K39" s="487"/>
       <c r="L39" s="117" t="s">
         <v>461</v>
       </c>
@@ -20510,14 +21229,14 @@
     </row>
     <row r="40" spans="1:14">
       <c r="C40" s="38"/>
-      <c r="D40" s="487"/>
-      <c r="E40" s="482"/>
-      <c r="F40" s="482"/>
-      <c r="G40" s="482"/>
-      <c r="H40" s="488"/>
-      <c r="I40" s="492"/>
-      <c r="J40" s="487"/>
-      <c r="K40" s="488"/>
+      <c r="D40" s="488"/>
+      <c r="E40" s="478"/>
+      <c r="F40" s="478"/>
+      <c r="G40" s="478"/>
+      <c r="H40" s="489"/>
+      <c r="I40" s="493"/>
+      <c r="J40" s="488"/>
+      <c r="K40" s="489"/>
       <c r="L40" s="483" t="s">
         <v>465</v>
       </c>
@@ -20526,14 +21245,14 @@
     </row>
     <row r="41" spans="1:14">
       <c r="C41" s="38"/>
-      <c r="D41" s="487"/>
-      <c r="E41" s="482"/>
-      <c r="F41" s="482"/>
-      <c r="G41" s="482"/>
-      <c r="H41" s="488"/>
-      <c r="I41" s="493"/>
-      <c r="J41" s="487"/>
-      <c r="K41" s="488"/>
+      <c r="D41" s="488"/>
+      <c r="E41" s="478"/>
+      <c r="F41" s="478"/>
+      <c r="G41" s="478"/>
+      <c r="H41" s="489"/>
+      <c r="I41" s="494"/>
+      <c r="J41" s="488"/>
+      <c r="K41" s="489"/>
       <c r="L41" s="118" t="s">
         <v>467</v>
       </c>
@@ -20542,16 +21261,16 @@
     </row>
     <row r="42" spans="1:14">
       <c r="C42" s="38"/>
-      <c r="D42" s="489"/>
+      <c r="D42" s="490"/>
       <c r="E42" s="470"/>
       <c r="F42" s="470"/>
       <c r="G42" s="470"/>
-      <c r="H42" s="490"/>
+      <c r="H42" s="491"/>
       <c r="I42" s="38" t="s">
         <v>458</v>
       </c>
-      <c r="J42" s="489"/>
-      <c r="K42" s="490"/>
+      <c r="J42" s="490"/>
+      <c r="K42" s="491"/>
       <c r="L42" s="119" t="s">
         <v>466</v>
       </c>
@@ -20863,12 +21582,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D39:H42"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="J39:K42"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="C34:C37"/>
+    <mergeCell ref="D34:H37"/>
+    <mergeCell ref="I34:I37"/>
+    <mergeCell ref="J34:K37"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="L36:N36"/>
     <mergeCell ref="C21:C24"/>
     <mergeCell ref="D21:H24"/>
     <mergeCell ref="J21:K24"/>
@@ -20876,17 +21600,12 @@
     <mergeCell ref="D26:H29"/>
     <mergeCell ref="I26:I29"/>
     <mergeCell ref="J26:K29"/>
-    <mergeCell ref="C34:C37"/>
-    <mergeCell ref="D34:H37"/>
-    <mergeCell ref="I34:I37"/>
-    <mergeCell ref="J34:K37"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D39:H42"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="J39:K42"/>
-    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="L21:N21"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="L23:N23"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="L27:N27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20908,29 +21627,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="21">
-      <c r="B2" s="517" t="s">
+      <c r="B2" s="508" t="s">
         <v>1075</v>
       </c>
-      <c r="C2" s="517"/>
-      <c r="D2" s="517"/>
-      <c r="E2" s="517"/>
-      <c r="F2" s="517"/>
-      <c r="G2" s="517"/>
-      <c r="H2" s="517"/>
-      <c r="I2" s="517"/>
-      <c r="J2" s="517"/>
-      <c r="K2" s="517"/>
-      <c r="L2" s="517"/>
-      <c r="M2" s="517"/>
-      <c r="N2" s="517"/>
-      <c r="O2" s="517"/>
-      <c r="P2" s="517"/>
-      <c r="Q2" s="517"/>
-      <c r="R2" s="517"/>
-      <c r="S2" s="517"/>
-      <c r="T2" s="517"/>
-      <c r="U2" s="517"/>
-      <c r="V2" s="517"/>
+      <c r="C2" s="508"/>
+      <c r="D2" s="508"/>
+      <c r="E2" s="508"/>
+      <c r="F2" s="508"/>
+      <c r="G2" s="508"/>
+      <c r="H2" s="508"/>
+      <c r="I2" s="508"/>
+      <c r="J2" s="508"/>
+      <c r="K2" s="508"/>
+      <c r="L2" s="508"/>
+      <c r="M2" s="508"/>
+      <c r="N2" s="508"/>
+      <c r="O2" s="508"/>
+      <c r="P2" s="508"/>
+      <c r="Q2" s="508"/>
+      <c r="R2" s="508"/>
+      <c r="S2" s="508"/>
+      <c r="T2" s="508"/>
+      <c r="U2" s="508"/>
+      <c r="V2" s="508"/>
     </row>
     <row r="3" spans="2:22" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:22">
@@ -20963,22 +21682,22 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="498" t="s">
+      <c r="G5" s="511" t="s">
         <v>518</v>
       </c>
-      <c r="H5" s="498"/>
-      <c r="I5" s="498" t="s">
+      <c r="H5" s="511"/>
+      <c r="I5" s="511" t="s">
         <v>519</v>
       </c>
-      <c r="J5" s="498"/>
-      <c r="K5" s="498"/>
-      <c r="L5" s="498"/>
-      <c r="M5" s="498"/>
-      <c r="N5" s="498"/>
-      <c r="O5" s="498" t="s">
+      <c r="J5" s="511"/>
+      <c r="K5" s="511"/>
+      <c r="L5" s="511"/>
+      <c r="M5" s="511"/>
+      <c r="N5" s="511"/>
+      <c r="O5" s="511" t="s">
         <v>520</v>
       </c>
-      <c r="P5" s="498"/>
+      <c r="P5" s="511"/>
       <c r="Q5" s="5"/>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
@@ -20990,7 +21709,7 @@
       <c r="D6" s="135"/>
       <c r="E6" s="136"/>
       <c r="F6" s="138"/>
-      <c r="G6" s="499" t="s">
+      <c r="G6" s="516" t="s">
         <v>521</v>
       </c>
       <c r="H6" s="111"/>
@@ -21020,25 +21739,25 @@
       <c r="E7" s="138"/>
       <c r="F7" s="138"/>
       <c r="G7" s="425"/>
-      <c r="H7" s="500" t="s">
+      <c r="H7" s="517" t="s">
         <v>523</v>
       </c>
-      <c r="I7" s="503" t="s">
+      <c r="I7" s="520" t="s">
         <v>524</v>
       </c>
-      <c r="J7" s="504"/>
-      <c r="K7" s="505" t="s">
+      <c r="J7" s="521"/>
+      <c r="K7" s="522" t="s">
         <v>525</v>
       </c>
-      <c r="L7" s="506"/>
-      <c r="M7" s="503" t="s">
+      <c r="L7" s="523"/>
+      <c r="M7" s="520" t="s">
         <v>526</v>
       </c>
-      <c r="N7" s="504"/>
-      <c r="O7" s="511" t="s">
+      <c r="N7" s="521"/>
+      <c r="O7" s="528" t="s">
         <v>527</v>
       </c>
-      <c r="P7" s="512"/>
+      <c r="P7" s="529"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -21051,15 +21770,15 @@
       <c r="E8" s="140"/>
       <c r="F8" s="138"/>
       <c r="G8" s="425"/>
-      <c r="H8" s="501"/>
+      <c r="H8" s="518"/>
       <c r="I8" s="420"/>
       <c r="J8" s="422"/>
-      <c r="K8" s="507"/>
-      <c r="L8" s="508"/>
+      <c r="K8" s="524"/>
+      <c r="L8" s="525"/>
       <c r="M8" s="420"/>
       <c r="N8" s="422"/>
-      <c r="O8" s="513"/>
-      <c r="P8" s="514"/>
+      <c r="O8" s="530"/>
+      <c r="P8" s="531"/>
       <c r="Q8" s="5"/>
       <c r="R8" s="38" t="s">
         <v>182</v>
@@ -21078,15 +21797,15 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="425"/>
-      <c r="H9" s="501"/>
+      <c r="H9" s="518"/>
       <c r="I9" s="420"/>
       <c r="J9" s="422"/>
-      <c r="K9" s="507"/>
-      <c r="L9" s="508"/>
+      <c r="K9" s="524"/>
+      <c r="L9" s="525"/>
       <c r="M9" s="420"/>
       <c r="N9" s="422"/>
-      <c r="O9" s="513"/>
-      <c r="P9" s="514"/>
+      <c r="O9" s="530"/>
+      <c r="P9" s="531"/>
       <c r="Q9" s="5" t="s">
         <v>2</v>
       </c>
@@ -21107,15 +21826,15 @@
       <c r="E10" s="3"/>
       <c r="F10" s="6"/>
       <c r="G10" s="425"/>
-      <c r="H10" s="501"/>
+      <c r="H10" s="518"/>
       <c r="I10" s="420"/>
       <c r="J10" s="422"/>
-      <c r="K10" s="507"/>
-      <c r="L10" s="508"/>
+      <c r="K10" s="524"/>
+      <c r="L10" s="525"/>
       <c r="M10" s="420"/>
       <c r="N10" s="422"/>
-      <c r="O10" s="513"/>
-      <c r="P10" s="514"/>
+      <c r="O10" s="530"/>
+      <c r="P10" s="531"/>
       <c r="Q10" s="5" t="s">
         <v>187</v>
       </c>
@@ -21132,15 +21851,15 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="425"/>
-      <c r="H11" s="501"/>
+      <c r="H11" s="518"/>
       <c r="I11" s="420"/>
       <c r="J11" s="422"/>
-      <c r="K11" s="507"/>
-      <c r="L11" s="508"/>
+      <c r="K11" s="524"/>
+      <c r="L11" s="525"/>
       <c r="M11" s="420"/>
       <c r="N11" s="422"/>
-      <c r="O11" s="513"/>
-      <c r="P11" s="514"/>
+      <c r="O11" s="530"/>
+      <c r="P11" s="531"/>
       <c r="Q11" s="5">
         <v>1000</v>
       </c>
@@ -21159,15 +21878,15 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="425"/>
-      <c r="H12" s="501"/>
+      <c r="H12" s="518"/>
       <c r="I12" s="420"/>
       <c r="J12" s="422"/>
-      <c r="K12" s="507"/>
-      <c r="L12" s="508"/>
+      <c r="K12" s="524"/>
+      <c r="L12" s="525"/>
       <c r="M12" s="420"/>
       <c r="N12" s="422"/>
-      <c r="O12" s="513"/>
-      <c r="P12" s="514"/>
+      <c r="O12" s="530"/>
+      <c r="P12" s="531"/>
       <c r="Q12" s="5" t="s">
         <v>2</v>
       </c>
@@ -21182,15 +21901,15 @@
       <c r="E13" s="9"/>
       <c r="F13" s="6"/>
       <c r="G13" s="425"/>
-      <c r="H13" s="501"/>
+      <c r="H13" s="518"/>
       <c r="I13" s="420"/>
       <c r="J13" s="422"/>
-      <c r="K13" s="507"/>
-      <c r="L13" s="508"/>
+      <c r="K13" s="524"/>
+      <c r="L13" s="525"/>
       <c r="M13" s="420"/>
       <c r="N13" s="422"/>
-      <c r="O13" s="513"/>
-      <c r="P13" s="514"/>
+      <c r="O13" s="530"/>
+      <c r="P13" s="531"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="38"/>
       <c r="S13" s="38"/>
@@ -21203,15 +21922,15 @@
       <c r="E14" s="3"/>
       <c r="F14" s="6"/>
       <c r="G14" s="425"/>
-      <c r="H14" s="501"/>
+      <c r="H14" s="518"/>
       <c r="I14" s="420"/>
       <c r="J14" s="422"/>
-      <c r="K14" s="507"/>
-      <c r="L14" s="508"/>
+      <c r="K14" s="524"/>
+      <c r="L14" s="525"/>
       <c r="M14" s="420"/>
       <c r="N14" s="422"/>
-      <c r="O14" s="513"/>
-      <c r="P14" s="514"/>
+      <c r="O14" s="530"/>
+      <c r="P14" s="531"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="38"/>
       <c r="S14" s="38"/>
@@ -21226,15 +21945,15 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="425"/>
-      <c r="H15" s="501"/>
+      <c r="H15" s="518"/>
       <c r="I15" s="420"/>
       <c r="J15" s="422"/>
-      <c r="K15" s="507"/>
-      <c r="L15" s="508"/>
+      <c r="K15" s="524"/>
+      <c r="L15" s="525"/>
       <c r="M15" s="420"/>
       <c r="N15" s="422"/>
-      <c r="O15" s="513"/>
-      <c r="P15" s="514"/>
+      <c r="O15" s="530"/>
+      <c r="P15" s="531"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
@@ -21247,15 +21966,15 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="425"/>
-      <c r="H16" s="501"/>
+      <c r="H16" s="518"/>
       <c r="I16" s="420"/>
       <c r="J16" s="422"/>
-      <c r="K16" s="507"/>
-      <c r="L16" s="508"/>
+      <c r="K16" s="524"/>
+      <c r="L16" s="525"/>
       <c r="M16" s="420"/>
       <c r="N16" s="422"/>
-      <c r="O16" s="513"/>
-      <c r="P16" s="514"/>
+      <c r="O16" s="530"/>
+      <c r="P16" s="531"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
@@ -21268,15 +21987,15 @@
       <c r="E17" s="9"/>
       <c r="F17" s="6"/>
       <c r="G17" s="425"/>
-      <c r="H17" s="501"/>
+      <c r="H17" s="518"/>
       <c r="I17" s="420"/>
       <c r="J17" s="422"/>
-      <c r="K17" s="507"/>
-      <c r="L17" s="508"/>
+      <c r="K17" s="524"/>
+      <c r="L17" s="525"/>
       <c r="M17" s="420"/>
       <c r="N17" s="422"/>
-      <c r="O17" s="513"/>
-      <c r="P17" s="514"/>
+      <c r="O17" s="530"/>
+      <c r="P17" s="531"/>
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
@@ -21289,15 +22008,15 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="425"/>
-      <c r="H18" s="501"/>
+      <c r="H18" s="518"/>
       <c r="I18" s="420"/>
       <c r="J18" s="422"/>
-      <c r="K18" s="507"/>
-      <c r="L18" s="508"/>
+      <c r="K18" s="524"/>
+      <c r="L18" s="525"/>
       <c r="M18" s="420"/>
       <c r="N18" s="422"/>
-      <c r="O18" s="513"/>
-      <c r="P18" s="514"/>
+      <c r="O18" s="530"/>
+      <c r="P18" s="531"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
@@ -21312,15 +22031,15 @@
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="425"/>
-      <c r="H19" s="501"/>
+      <c r="H19" s="518"/>
       <c r="I19" s="420"/>
       <c r="J19" s="422"/>
-      <c r="K19" s="507"/>
-      <c r="L19" s="508"/>
+      <c r="K19" s="524"/>
+      <c r="L19" s="525"/>
       <c r="M19" s="420"/>
       <c r="N19" s="422"/>
-      <c r="O19" s="513"/>
-      <c r="P19" s="514"/>
+      <c r="O19" s="530"/>
+      <c r="P19" s="531"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
@@ -21333,15 +22052,15 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="426"/>
-      <c r="H20" s="502"/>
+      <c r="H20" s="519"/>
       <c r="I20" s="441"/>
       <c r="J20" s="443"/>
-      <c r="K20" s="509"/>
-      <c r="L20" s="510"/>
+      <c r="K20" s="526"/>
+      <c r="L20" s="527"/>
       <c r="M20" s="441"/>
       <c r="N20" s="443"/>
-      <c r="O20" s="515"/>
-      <c r="P20" s="516"/>
+      <c r="O20" s="532"/>
+      <c r="P20" s="533"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
@@ -21422,49 +22141,49 @@
       <c r="U23" s="9"/>
     </row>
     <row r="25" spans="2:22" ht="21">
-      <c r="B25" s="517" t="s">
+      <c r="B25" s="508" t="s">
         <v>1074</v>
       </c>
-      <c r="C25" s="517"/>
-      <c r="D25" s="517"/>
-      <c r="E25" s="517"/>
-      <c r="F25" s="517"/>
-      <c r="G25" s="517"/>
-      <c r="H25" s="517"/>
-      <c r="I25" s="517"/>
-      <c r="J25" s="517"/>
-      <c r="K25" s="517"/>
-      <c r="L25" s="517"/>
-      <c r="M25" s="517"/>
-      <c r="N25" s="517"/>
-      <c r="O25" s="517"/>
-      <c r="P25" s="517"/>
-      <c r="Q25" s="517"/>
-      <c r="R25" s="517"/>
-      <c r="S25" s="517"/>
-      <c r="T25" s="517"/>
-      <c r="U25" s="517"/>
-      <c r="V25" s="517"/>
+      <c r="C25" s="508"/>
+      <c r="D25" s="508"/>
+      <c r="E25" s="508"/>
+      <c r="F25" s="508"/>
+      <c r="G25" s="508"/>
+      <c r="H25" s="508"/>
+      <c r="I25" s="508"/>
+      <c r="J25" s="508"/>
+      <c r="K25" s="508"/>
+      <c r="L25" s="508"/>
+      <c r="M25" s="508"/>
+      <c r="N25" s="508"/>
+      <c r="O25" s="508"/>
+      <c r="P25" s="508"/>
+      <c r="Q25" s="508"/>
+      <c r="R25" s="508"/>
+      <c r="S25" s="508"/>
+      <c r="T25" s="508"/>
+      <c r="U25" s="508"/>
+      <c r="V25" s="508"/>
     </row>
     <row r="26" spans="2:22" ht="15.75" thickBot="1">
-      <c r="C26" s="518" t="s">
+      <c r="C26" s="509" t="s">
         <v>570</v>
       </c>
-      <c r="D26" s="518"/>
-      <c r="E26" s="518"/>
-      <c r="F26" s="518"/>
-      <c r="G26" s="518"/>
-      <c r="H26" s="518"/>
-      <c r="I26" s="518"/>
-      <c r="J26" s="518"/>
-      <c r="K26" s="518"/>
-      <c r="L26" s="518"/>
-      <c r="M26" s="518"/>
+      <c r="D26" s="509"/>
+      <c r="E26" s="509"/>
+      <c r="F26" s="509"/>
+      <c r="G26" s="509"/>
+      <c r="H26" s="509"/>
+      <c r="I26" s="509"/>
+      <c r="J26" s="509"/>
+      <c r="K26" s="509"/>
+      <c r="L26" s="509"/>
+      <c r="M26" s="509"/>
     </row>
     <row r="27" spans="2:22" ht="15.75" thickBot="1">
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="472" t="s">
+      <c r="E27" s="479" t="s">
         <v>178</v>
       </c>
       <c r="F27" s="416"/>
@@ -21507,11 +22226,11 @@
       <c r="K29" s="4"/>
       <c r="L29" s="5"/>
       <c r="M29" s="6"/>
-      <c r="O29" s="519" t="s">
+      <c r="O29" s="510" t="s">
         <v>179</v>
       </c>
-      <c r="P29" s="519"/>
-      <c r="Q29" s="519"/>
+      <c r="P29" s="510"/>
+      <c r="Q29" s="510"/>
     </row>
     <row r="30" spans="2:22" ht="15.75" thickBot="1">
       <c r="C30" s="4"/>
@@ -21556,21 +22275,21 @@
         <v>190</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="523" t="s">
+      <c r="E32" s="505" t="s">
         <v>1078</v>
       </c>
-      <c r="F32" s="524"/>
-      <c r="G32" s="525"/>
-      <c r="H32" s="523" t="s">
+      <c r="F32" s="506"/>
+      <c r="G32" s="507"/>
+      <c r="H32" s="505" t="s">
         <v>1079</v>
       </c>
-      <c r="I32" s="524"/>
-      <c r="J32" s="525"/>
-      <c r="K32" s="523" t="s">
+      <c r="I32" s="506"/>
+      <c r="J32" s="507"/>
+      <c r="K32" s="505" t="s">
         <v>1080</v>
       </c>
-      <c r="L32" s="524"/>
-      <c r="M32" s="525"/>
+      <c r="L32" s="506"/>
+      <c r="M32" s="507"/>
       <c r="N32" s="5" t="s">
         <v>2</v>
       </c>
@@ -21587,15 +22306,15 @@
     <row r="33" spans="2:22">
       <c r="C33" s="4"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="523"/>
-      <c r="F33" s="524"/>
-      <c r="G33" s="525"/>
-      <c r="H33" s="523"/>
-      <c r="I33" s="524"/>
-      <c r="J33" s="525"/>
-      <c r="K33" s="523"/>
-      <c r="L33" s="524"/>
-      <c r="M33" s="525"/>
+      <c r="E33" s="505"/>
+      <c r="F33" s="506"/>
+      <c r="G33" s="507"/>
+      <c r="H33" s="505"/>
+      <c r="I33" s="506"/>
+      <c r="J33" s="507"/>
+      <c r="K33" s="505"/>
+      <c r="L33" s="506"/>
+      <c r="M33" s="507"/>
       <c r="N33" s="5" t="s">
         <v>187</v>
       </c>
@@ -21612,15 +22331,15 @@
     <row r="34" spans="2:22" ht="15.75" thickBot="1">
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="523"/>
-      <c r="F34" s="524"/>
-      <c r="G34" s="525"/>
-      <c r="H34" s="523"/>
-      <c r="I34" s="524"/>
-      <c r="J34" s="525"/>
-      <c r="K34" s="523"/>
-      <c r="L34" s="524"/>
-      <c r="M34" s="525"/>
+      <c r="E34" s="505"/>
+      <c r="F34" s="506"/>
+      <c r="G34" s="507"/>
+      <c r="H34" s="505"/>
+      <c r="I34" s="506"/>
+      <c r="J34" s="507"/>
+      <c r="K34" s="505"/>
+      <c r="L34" s="506"/>
+      <c r="M34" s="507"/>
       <c r="N34" s="5">
         <v>1000</v>
       </c>
@@ -21631,15 +22350,15 @@
     <row r="35" spans="2:22">
       <c r="C35" s="1"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="523"/>
-      <c r="F35" s="524"/>
-      <c r="G35" s="525"/>
-      <c r="H35" s="523"/>
-      <c r="I35" s="524"/>
-      <c r="J35" s="525"/>
-      <c r="K35" s="523"/>
-      <c r="L35" s="524"/>
-      <c r="M35" s="525"/>
+      <c r="E35" s="505"/>
+      <c r="F35" s="506"/>
+      <c r="G35" s="507"/>
+      <c r="H35" s="505"/>
+      <c r="I35" s="506"/>
+      <c r="J35" s="507"/>
+      <c r="K35" s="505"/>
+      <c r="L35" s="506"/>
+      <c r="M35" s="507"/>
       <c r="N35" s="5" t="s">
         <v>2</v>
       </c>
@@ -21770,15 +22489,15 @@
     <row r="42" spans="2:22" ht="19.5" thickBot="1">
       <c r="C42" s="8"/>
       <c r="D42" s="9"/>
-      <c r="E42" s="527"/>
-      <c r="F42" s="528"/>
-      <c r="G42" s="528"/>
-      <c r="H42" s="528"/>
-      <c r="I42" s="528"/>
-      <c r="J42" s="528"/>
-      <c r="K42" s="528"/>
-      <c r="L42" s="528"/>
-      <c r="M42" s="529"/>
+      <c r="E42" s="498"/>
+      <c r="F42" s="499"/>
+      <c r="G42" s="499"/>
+      <c r="H42" s="499"/>
+      <c r="I42" s="499"/>
+      <c r="J42" s="499"/>
+      <c r="K42" s="499"/>
+      <c r="L42" s="499"/>
+      <c r="M42" s="500"/>
       <c r="N42" s="40" t="s">
         <v>575</v>
       </c>
@@ -21819,51 +22538,51 @@
       </c>
     </row>
     <row r="47" spans="2:22" ht="21">
-      <c r="B47" s="517" t="s">
+      <c r="B47" s="508" t="s">
         <v>1076</v>
       </c>
-      <c r="C47" s="517"/>
-      <c r="D47" s="517"/>
-      <c r="E47" s="517"/>
-      <c r="F47" s="517"/>
-      <c r="G47" s="517"/>
-      <c r="H47" s="517"/>
-      <c r="I47" s="517"/>
-      <c r="J47" s="517"/>
-      <c r="K47" s="517"/>
-      <c r="L47" s="517"/>
-      <c r="M47" s="517"/>
-      <c r="N47" s="517"/>
-      <c r="O47" s="517"/>
-      <c r="P47" s="517"/>
-      <c r="Q47" s="517"/>
-      <c r="R47" s="517"/>
-      <c r="S47" s="517"/>
-      <c r="T47" s="517"/>
-      <c r="U47" s="517"/>
-      <c r="V47" s="517"/>
+      <c r="C47" s="508"/>
+      <c r="D47" s="508"/>
+      <c r="E47" s="508"/>
+      <c r="F47" s="508"/>
+      <c r="G47" s="508"/>
+      <c r="H47" s="508"/>
+      <c r="I47" s="508"/>
+      <c r="J47" s="508"/>
+      <c r="K47" s="508"/>
+      <c r="L47" s="508"/>
+      <c r="M47" s="508"/>
+      <c r="N47" s="508"/>
+      <c r="O47" s="508"/>
+      <c r="P47" s="508"/>
+      <c r="Q47" s="508"/>
+      <c r="R47" s="508"/>
+      <c r="S47" s="508"/>
+      <c r="T47" s="508"/>
+      <c r="U47" s="508"/>
+      <c r="V47" s="508"/>
     </row>
     <row r="48" spans="2:22" ht="15.75" thickBot="1">
-      <c r="C48" s="518" t="s">
+      <c r="C48" s="509" t="s">
         <v>570</v>
       </c>
-      <c r="D48" s="518"/>
-      <c r="E48" s="518"/>
-      <c r="F48" s="518"/>
-      <c r="G48" s="518"/>
-      <c r="H48" s="518"/>
-      <c r="I48" s="518"/>
-      <c r="J48" s="518"/>
-      <c r="K48" s="518"/>
-      <c r="L48" s="518"/>
-      <c r="M48" s="518"/>
+      <c r="D48" s="509"/>
+      <c r="E48" s="509"/>
+      <c r="F48" s="509"/>
+      <c r="G48" s="509"/>
+      <c r="H48" s="509"/>
+      <c r="I48" s="509"/>
+      <c r="J48" s="509"/>
+      <c r="K48" s="509"/>
+      <c r="L48" s="509"/>
+      <c r="M48" s="509"/>
       <c r="S48" s="24"/>
       <c r="T48" s="24"/>
     </row>
     <row r="49" spans="1:24" ht="15.75" thickBot="1">
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="472" t="s">
+      <c r="E49" s="479" t="s">
         <v>178</v>
       </c>
       <c r="F49" s="416"/>
@@ -21891,16 +22610,16 @@
       </c>
       <c r="F50" s="122"/>
       <c r="G50" s="245"/>
-      <c r="H50" s="520" t="s">
+      <c r="H50" s="512" t="s">
         <v>1079</v>
       </c>
-      <c r="I50" s="521"/>
-      <c r="J50" s="522"/>
-      <c r="K50" s="520" t="s">
+      <c r="I50" s="513"/>
+      <c r="J50" s="514"/>
+      <c r="K50" s="512" t="s">
         <v>1080</v>
       </c>
-      <c r="L50" s="521"/>
-      <c r="M50" s="522"/>
+      <c r="L50" s="513"/>
+      <c r="M50" s="514"/>
       <c r="S50" s="24"/>
       <c r="T50" s="24"/>
       <c r="W50" t="s">
@@ -21914,20 +22633,20 @@
         <v>1094</v>
       </c>
       <c r="F51" s="286"/>
-      <c r="G51" s="526" t="s">
+      <c r="G51" s="515" t="s">
         <v>1102</v>
       </c>
-      <c r="H51" s="523"/>
-      <c r="I51" s="524"/>
-      <c r="J51" s="525"/>
-      <c r="K51" s="523"/>
-      <c r="L51" s="524"/>
-      <c r="M51" s="525"/>
-      <c r="O51" s="519" t="s">
+      <c r="H51" s="505"/>
+      <c r="I51" s="506"/>
+      <c r="J51" s="507"/>
+      <c r="K51" s="505"/>
+      <c r="L51" s="506"/>
+      <c r="M51" s="507"/>
+      <c r="O51" s="510" t="s">
         <v>179</v>
       </c>
-      <c r="P51" s="519"/>
-      <c r="Q51" s="519"/>
+      <c r="P51" s="510"/>
+      <c r="Q51" s="510"/>
       <c r="S51" s="273"/>
       <c r="T51" s="273"/>
       <c r="W51" s="40" t="s">
@@ -21941,13 +22660,13 @@
         <v>1095</v>
       </c>
       <c r="F52" s="287"/>
-      <c r="G52" s="526"/>
-      <c r="H52" s="523"/>
-      <c r="I52" s="524"/>
-      <c r="J52" s="525"/>
-      <c r="K52" s="523"/>
-      <c r="L52" s="524"/>
-      <c r="M52" s="525"/>
+      <c r="G52" s="515"/>
+      <c r="H52" s="505"/>
+      <c r="I52" s="506"/>
+      <c r="J52" s="507"/>
+      <c r="K52" s="505"/>
+      <c r="L52" s="506"/>
+      <c r="M52" s="507"/>
       <c r="S52" s="24"/>
       <c r="T52" s="24"/>
     </row>
@@ -21958,13 +22677,13 @@
         <v>1096</v>
       </c>
       <c r="F53" s="288"/>
-      <c r="G53" s="526"/>
-      <c r="H53" s="523"/>
-      <c r="I53" s="524"/>
-      <c r="J53" s="525"/>
-      <c r="K53" s="523"/>
-      <c r="L53" s="524"/>
-      <c r="M53" s="525"/>
+      <c r="G53" s="515"/>
+      <c r="H53" s="505"/>
+      <c r="I53" s="506"/>
+      <c r="J53" s="507"/>
+      <c r="K53" s="505"/>
+      <c r="L53" s="506"/>
+      <c r="M53" s="507"/>
       <c r="N53" s="5"/>
       <c r="O53" s="38" t="s">
         <v>182</v>
@@ -22003,7 +22722,7 @@
       <c r="D54" s="6"/>
       <c r="E54" s="274"/>
       <c r="F54" s="289"/>
-      <c r="G54" s="532" t="s">
+      <c r="G54" s="503" t="s">
         <v>1106</v>
       </c>
       <c r="H54" s="4" t="s">
@@ -22050,11 +22769,11 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="6"/>
-      <c r="E55" s="530" t="s">
+      <c r="E55" s="501" t="s">
         <v>1107</v>
       </c>
-      <c r="F55" s="531"/>
-      <c r="G55" s="533"/>
+      <c r="F55" s="502"/>
+      <c r="G55" s="504"/>
       <c r="H55" s="141" t="s">
         <v>1098</v>
       </c>
@@ -22098,9 +22817,9 @@
     <row r="56" spans="1:24" ht="15.75" customHeight="1" thickBot="1">
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="530"/>
-      <c r="F56" s="531"/>
-      <c r="G56" s="533"/>
+      <c r="E56" s="501"/>
+      <c r="F56" s="502"/>
+      <c r="G56" s="504"/>
       <c r="H56" s="141" t="s">
         <v>1099</v>
       </c>
@@ -22130,9 +22849,9 @@
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="530"/>
-      <c r="F57" s="531"/>
-      <c r="G57" s="533"/>
+      <c r="E57" s="501"/>
+      <c r="F57" s="502"/>
+      <c r="G57" s="504"/>
       <c r="H57" s="4" t="s">
         <v>1111</v>
       </c>
@@ -22162,9 +22881,9 @@
         <v>192</v>
       </c>
       <c r="D58" s="6"/>
-      <c r="E58" s="530"/>
-      <c r="F58" s="531"/>
-      <c r="G58" s="533"/>
+      <c r="E58" s="501"/>
+      <c r="F58" s="502"/>
+      <c r="G58" s="504"/>
       <c r="H58" s="278" t="s">
         <v>1097</v>
       </c>
@@ -22189,9 +22908,9 @@
     <row r="59" spans="1:24">
       <c r="C59" s="4"/>
       <c r="D59" s="6"/>
-      <c r="E59" s="530"/>
-      <c r="F59" s="531"/>
-      <c r="G59" s="533"/>
+      <c r="E59" s="501"/>
+      <c r="F59" s="502"/>
+      <c r="G59" s="504"/>
       <c r="H59" s="278" t="s">
         <v>549</v>
       </c>
@@ -22216,9 +22935,9 @@
     <row r="60" spans="1:24" ht="15.75" thickBot="1">
       <c r="C60" s="8"/>
       <c r="D60" s="9"/>
-      <c r="E60" s="530"/>
-      <c r="F60" s="531"/>
-      <c r="G60" s="533"/>
+      <c r="E60" s="501"/>
+      <c r="F60" s="502"/>
+      <c r="G60" s="504"/>
       <c r="H60" s="280"/>
       <c r="I60" s="281" t="s">
         <v>1113</v>
@@ -22238,9 +22957,9 @@
     <row r="61" spans="1:24">
       <c r="C61" s="4"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="530"/>
-      <c r="F61" s="531"/>
-      <c r="G61" s="533"/>
+      <c r="E61" s="501"/>
+      <c r="F61" s="502"/>
+      <c r="G61" s="504"/>
       <c r="H61" s="280"/>
       <c r="I61" s="281" t="s">
         <v>1114</v>
@@ -22260,7 +22979,7 @@
       <c r="D62" s="6"/>
       <c r="E62" s="269"/>
       <c r="F62" s="285"/>
-      <c r="G62" s="533"/>
+      <c r="G62" s="504"/>
       <c r="H62" s="282"/>
       <c r="I62" s="284" t="s">
         <v>1115</v>
@@ -22302,15 +23021,15 @@
     <row r="64" spans="1:24" ht="19.5" thickBot="1">
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
-      <c r="E64" s="527"/>
-      <c r="F64" s="528"/>
-      <c r="G64" s="528"/>
-      <c r="H64" s="528"/>
-      <c r="I64" s="528"/>
-      <c r="J64" s="528"/>
-      <c r="K64" s="528"/>
-      <c r="L64" s="528"/>
-      <c r="M64" s="529"/>
+      <c r="E64" s="498"/>
+      <c r="F64" s="499"/>
+      <c r="G64" s="499"/>
+      <c r="H64" s="499"/>
+      <c r="I64" s="499"/>
+      <c r="J64" s="499"/>
+      <c r="K64" s="499"/>
+      <c r="L64" s="499"/>
+      <c r="M64" s="500"/>
       <c r="N64" s="40" t="s">
         <v>575</v>
       </c>
@@ -23189,30 +23908,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E64:M64"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="H66:M66"/>
-    <mergeCell ref="E55:F61"/>
-    <mergeCell ref="G54:G62"/>
-    <mergeCell ref="E32:G35"/>
-    <mergeCell ref="H32:J35"/>
-    <mergeCell ref="K32:M35"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="H22:N22"/>
-    <mergeCell ref="B2:V2"/>
-    <mergeCell ref="B25:V25"/>
-    <mergeCell ref="C26:M26"/>
-    <mergeCell ref="E27:M27"/>
-    <mergeCell ref="O29:Q29"/>
-    <mergeCell ref="O22:P22"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K50:M53"/>
-    <mergeCell ref="G51:G53"/>
-    <mergeCell ref="E42:M42"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:M44"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="E68:G68"/>
     <mergeCell ref="H68:M68"/>
@@ -23229,6 +23924,30 @@
     <mergeCell ref="E49:M49"/>
     <mergeCell ref="O51:Q51"/>
     <mergeCell ref="H50:J53"/>
+    <mergeCell ref="K50:M53"/>
+    <mergeCell ref="G51:G53"/>
+    <mergeCell ref="E42:M42"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:M44"/>
+    <mergeCell ref="B2:V2"/>
+    <mergeCell ref="B25:V25"/>
+    <mergeCell ref="C26:M26"/>
+    <mergeCell ref="E27:M27"/>
+    <mergeCell ref="O29:Q29"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E32:G35"/>
+    <mergeCell ref="H32:J35"/>
+    <mergeCell ref="K32:M35"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="H22:N22"/>
+    <mergeCell ref="E64:M64"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="H66:M66"/>
+    <mergeCell ref="E55:F61"/>
+    <mergeCell ref="G54:G62"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="T9" r:id="rId1"/>
@@ -23384,12 +24103,12 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="B8" s="482" t="s">
+      <c r="B8" s="478" t="s">
         <v>1401</v>
       </c>
-      <c r="C8" s="482"/>
-      <c r="D8" s="482"/>
-      <c r="E8" s="482"/>
+      <c r="C8" s="478"/>
+      <c r="D8" s="478"/>
+      <c r="E8" s="478"/>
       <c r="J8" s="32" t="s">
         <v>554</v>
       </c>
@@ -23562,23 +24281,23 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" thickBot="1">
-      <c r="C2" s="518" t="s">
+      <c r="C2" s="509" t="s">
         <v>570</v>
       </c>
-      <c r="D2" s="518"/>
-      <c r="E2" s="518"/>
-      <c r="F2" s="518"/>
-      <c r="G2" s="518"/>
-      <c r="H2" s="518"/>
-      <c r="I2" s="518"/>
-      <c r="J2" s="518"/>
-      <c r="K2" s="518"/>
-      <c r="L2" s="518"/>
+      <c r="D2" s="509"/>
+      <c r="E2" s="509"/>
+      <c r="F2" s="509"/>
+      <c r="G2" s="509"/>
+      <c r="H2" s="509"/>
+      <c r="I2" s="509"/>
+      <c r="J2" s="509"/>
+      <c r="K2" s="509"/>
+      <c r="L2" s="509"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="C3" s="1"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="472" t="s">
+      <c r="E3" s="479" t="s">
         <v>178</v>
       </c>
       <c r="F3" s="416"/>
@@ -23618,11 +24337,11 @@
         <v>589</v>
       </c>
       <c r="L5" s="6"/>
-      <c r="N5" s="519" t="s">
+      <c r="N5" s="510" t="s">
         <v>179</v>
       </c>
-      <c r="O5" s="519"/>
-      <c r="P5" s="519"/>
+      <c r="O5" s="510"/>
+      <c r="P5" s="510"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" thickBot="1">
       <c r="C6" s="4"/>
@@ -23673,20 +24392,20 @@
         <v>190</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="523" t="s">
+      <c r="E8" s="505" t="s">
         <v>571</v>
       </c>
-      <c r="F8" s="525"/>
-      <c r="G8" s="523" t="s">
+      <c r="F8" s="507"/>
+      <c r="G8" s="505" t="s">
         <v>572</v>
       </c>
-      <c r="H8" s="524"/>
-      <c r="I8" s="525"/>
-      <c r="J8" s="523" t="s">
+      <c r="H8" s="506"/>
+      <c r="I8" s="507"/>
+      <c r="J8" s="505" t="s">
         <v>573</v>
       </c>
-      <c r="K8" s="524"/>
-      <c r="L8" s="525"/>
+      <c r="K8" s="506"/>
+      <c r="L8" s="507"/>
       <c r="M8" s="5" t="s">
         <v>2</v>
       </c>
@@ -23709,14 +24428,14 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="523"/>
-      <c r="F9" s="525"/>
-      <c r="G9" s="523"/>
-      <c r="H9" s="524"/>
-      <c r="I9" s="525"/>
-      <c r="J9" s="523"/>
-      <c r="K9" s="524"/>
-      <c r="L9" s="525"/>
+      <c r="E9" s="505"/>
+      <c r="F9" s="507"/>
+      <c r="G9" s="505"/>
+      <c r="H9" s="506"/>
+      <c r="I9" s="507"/>
+      <c r="J9" s="505"/>
+      <c r="K9" s="506"/>
+      <c r="L9" s="507"/>
       <c r="M9" s="5" t="s">
         <v>187</v>
       </c>
@@ -23736,14 +24455,14 @@
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="523"/>
-      <c r="F10" s="525"/>
-      <c r="G10" s="523"/>
-      <c r="H10" s="524"/>
-      <c r="I10" s="525"/>
-      <c r="J10" s="523"/>
-      <c r="K10" s="524"/>
-      <c r="L10" s="525"/>
+      <c r="E10" s="505"/>
+      <c r="F10" s="507"/>
+      <c r="G10" s="505"/>
+      <c r="H10" s="506"/>
+      <c r="I10" s="507"/>
+      <c r="J10" s="505"/>
+      <c r="K10" s="506"/>
+      <c r="L10" s="507"/>
       <c r="M10" s="5">
         <v>1000</v>
       </c>
@@ -23757,14 +24476,14 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="523"/>
-      <c r="F11" s="525"/>
-      <c r="G11" s="523"/>
-      <c r="H11" s="524"/>
-      <c r="I11" s="525"/>
-      <c r="J11" s="523"/>
-      <c r="K11" s="524"/>
-      <c r="L11" s="525"/>
+      <c r="E11" s="505"/>
+      <c r="F11" s="507"/>
+      <c r="G11" s="505"/>
+      <c r="H11" s="506"/>
+      <c r="I11" s="507"/>
+      <c r="J11" s="505"/>
+      <c r="K11" s="506"/>
+      <c r="L11" s="507"/>
       <c r="M11" s="5" t="s">
         <v>2</v>
       </c>
@@ -23867,16 +24586,16 @@
     <row r="17" spans="3:15" ht="19.5" thickBot="1">
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="527" t="s">
+      <c r="E17" s="498" t="s">
         <v>574</v>
       </c>
-      <c r="F17" s="528"/>
-      <c r="G17" s="528"/>
-      <c r="H17" s="528"/>
-      <c r="I17" s="528"/>
-      <c r="J17" s="528"/>
-      <c r="K17" s="528"/>
-      <c r="L17" s="529"/>
+      <c r="F17" s="499"/>
+      <c r="G17" s="499"/>
+      <c r="H17" s="499"/>
+      <c r="I17" s="499"/>
+      <c r="J17" s="499"/>
+      <c r="K17" s="499"/>
+      <c r="L17" s="500"/>
       <c r="M17" s="40" t="s">
         <v>575</v>
       </c>
@@ -24395,22 +25114,22 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="498" t="s">
+      <c r="E3" s="511" t="s">
         <v>518</v>
       </c>
-      <c r="F3" s="498"/>
-      <c r="G3" s="498" t="s">
+      <c r="F3" s="511"/>
+      <c r="G3" s="511" t="s">
         <v>519</v>
       </c>
-      <c r="H3" s="498"/>
-      <c r="I3" s="498"/>
-      <c r="J3" s="498"/>
-      <c r="K3" s="498"/>
-      <c r="L3" s="498"/>
-      <c r="M3" s="498" t="s">
+      <c r="H3" s="511"/>
+      <c r="I3" s="511"/>
+      <c r="J3" s="511"/>
+      <c r="K3" s="511"/>
+      <c r="L3" s="511"/>
+      <c r="M3" s="511" t="s">
         <v>520</v>
       </c>
-      <c r="N3" s="498"/>
+      <c r="N3" s="511"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -24421,7 +25140,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="135"/>
       <c r="D4" s="136"/>
-      <c r="E4" s="499" t="s">
+      <c r="E4" s="516" t="s">
         <v>521</v>
       </c>
       <c r="F4" s="131"/>
@@ -24455,16 +25174,16 @@
       </c>
       <c r="G5" s="458"/>
       <c r="H5" s="459"/>
-      <c r="I5" s="571" t="s">
+      <c r="I5" s="541" t="s">
         <v>618</v>
       </c>
-      <c r="J5" s="572"/>
-      <c r="K5" s="572"/>
-      <c r="L5" s="506"/>
-      <c r="M5" s="571" t="s">
+      <c r="J5" s="542"/>
+      <c r="K5" s="542"/>
+      <c r="L5" s="523"/>
+      <c r="M5" s="541" t="s">
         <v>619</v>
       </c>
-      <c r="N5" s="506"/>
+      <c r="N5" s="523"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -24479,12 +25198,12 @@
       <c r="F6" s="460"/>
       <c r="G6" s="461"/>
       <c r="H6" s="462"/>
-      <c r="I6" s="507"/>
-      <c r="J6" s="573"/>
-      <c r="K6" s="573"/>
-      <c r="L6" s="508"/>
-      <c r="M6" s="507"/>
-      <c r="N6" s="508"/>
+      <c r="I6" s="524"/>
+      <c r="J6" s="543"/>
+      <c r="K6" s="543"/>
+      <c r="L6" s="525"/>
+      <c r="M6" s="524"/>
+      <c r="N6" s="525"/>
       <c r="O6" s="5"/>
       <c r="P6" s="38" t="s">
         <v>182</v>
@@ -24505,12 +25224,12 @@
       <c r="F7" s="460"/>
       <c r="G7" s="461"/>
       <c r="H7" s="462"/>
-      <c r="I7" s="507"/>
-      <c r="J7" s="573"/>
-      <c r="K7" s="573"/>
-      <c r="L7" s="508"/>
-      <c r="M7" s="507"/>
-      <c r="N7" s="508"/>
+      <c r="I7" s="524"/>
+      <c r="J7" s="543"/>
+      <c r="K7" s="543"/>
+      <c r="L7" s="525"/>
+      <c r="M7" s="524"/>
+      <c r="N7" s="525"/>
       <c r="O7" s="5" t="s">
         <v>2</v>
       </c>
@@ -24533,12 +25252,12 @@
       <c r="F8" s="460"/>
       <c r="G8" s="461"/>
       <c r="H8" s="462"/>
-      <c r="I8" s="507"/>
-      <c r="J8" s="573"/>
-      <c r="K8" s="573"/>
-      <c r="L8" s="508"/>
-      <c r="M8" s="507"/>
-      <c r="N8" s="508"/>
+      <c r="I8" s="524"/>
+      <c r="J8" s="543"/>
+      <c r="K8" s="543"/>
+      <c r="L8" s="525"/>
+      <c r="M8" s="524"/>
+      <c r="N8" s="525"/>
       <c r="O8" s="5" t="s">
         <v>187</v>
       </c>
@@ -24563,12 +25282,12 @@
       <c r="F9" s="460"/>
       <c r="G9" s="461"/>
       <c r="H9" s="462"/>
-      <c r="I9" s="507"/>
-      <c r="J9" s="573"/>
-      <c r="K9" s="573"/>
-      <c r="L9" s="508"/>
-      <c r="M9" s="507"/>
-      <c r="N9" s="508"/>
+      <c r="I9" s="524"/>
+      <c r="J9" s="543"/>
+      <c r="K9" s="543"/>
+      <c r="L9" s="525"/>
+      <c r="M9" s="524"/>
+      <c r="N9" s="525"/>
       <c r="O9" s="5">
         <v>1000</v>
       </c>
@@ -24589,12 +25308,12 @@
       <c r="F10" s="460"/>
       <c r="G10" s="461"/>
       <c r="H10" s="462"/>
-      <c r="I10" s="507"/>
-      <c r="J10" s="573"/>
-      <c r="K10" s="573"/>
-      <c r="L10" s="508"/>
-      <c r="M10" s="507"/>
-      <c r="N10" s="508"/>
+      <c r="I10" s="524"/>
+      <c r="J10" s="543"/>
+      <c r="K10" s="543"/>
+      <c r="L10" s="525"/>
+      <c r="M10" s="524"/>
+      <c r="N10" s="525"/>
       <c r="O10" s="5" t="s">
         <v>2</v>
       </c>
@@ -24611,12 +25330,12 @@
       <c r="F11" s="460"/>
       <c r="G11" s="461"/>
       <c r="H11" s="462"/>
-      <c r="I11" s="507"/>
-      <c r="J11" s="573"/>
-      <c r="K11" s="573"/>
-      <c r="L11" s="508"/>
-      <c r="M11" s="507"/>
-      <c r="N11" s="508"/>
+      <c r="I11" s="524"/>
+      <c r="J11" s="543"/>
+      <c r="K11" s="543"/>
+      <c r="L11" s="525"/>
+      <c r="M11" s="524"/>
+      <c r="N11" s="525"/>
       <c r="O11" s="5"/>
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
@@ -24631,12 +25350,12 @@
       <c r="F12" s="460"/>
       <c r="G12" s="461"/>
       <c r="H12" s="462"/>
-      <c r="I12" s="507"/>
-      <c r="J12" s="573"/>
-      <c r="K12" s="573"/>
-      <c r="L12" s="508"/>
-      <c r="M12" s="507"/>
-      <c r="N12" s="508"/>
+      <c r="I12" s="524"/>
+      <c r="J12" s="543"/>
+      <c r="K12" s="543"/>
+      <c r="L12" s="525"/>
+      <c r="M12" s="524"/>
+      <c r="N12" s="525"/>
       <c r="O12" s="5"/>
       <c r="P12" s="38"/>
       <c r="Q12" s="38"/>
@@ -24653,12 +25372,12 @@
       <c r="F13" s="460"/>
       <c r="G13" s="461"/>
       <c r="H13" s="462"/>
-      <c r="I13" s="507"/>
-      <c r="J13" s="573"/>
-      <c r="K13" s="573"/>
-      <c r="L13" s="508"/>
-      <c r="M13" s="507"/>
-      <c r="N13" s="508"/>
+      <c r="I13" s="524"/>
+      <c r="J13" s="543"/>
+      <c r="K13" s="543"/>
+      <c r="L13" s="525"/>
+      <c r="M13" s="524"/>
+      <c r="N13" s="525"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
@@ -24673,12 +25392,12 @@
       <c r="F14" s="460"/>
       <c r="G14" s="461"/>
       <c r="H14" s="462"/>
-      <c r="I14" s="507"/>
-      <c r="J14" s="573"/>
-      <c r="K14" s="573"/>
-      <c r="L14" s="508"/>
-      <c r="M14" s="507"/>
-      <c r="N14" s="508"/>
+      <c r="I14" s="524"/>
+      <c r="J14" s="543"/>
+      <c r="K14" s="543"/>
+      <c r="L14" s="525"/>
+      <c r="M14" s="524"/>
+      <c r="N14" s="525"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
@@ -24693,12 +25412,12 @@
       <c r="F15" s="460"/>
       <c r="G15" s="461"/>
       <c r="H15" s="462"/>
-      <c r="I15" s="507"/>
-      <c r="J15" s="573"/>
-      <c r="K15" s="573"/>
-      <c r="L15" s="508"/>
-      <c r="M15" s="507"/>
-      <c r="N15" s="508"/>
+      <c r="I15" s="524"/>
+      <c r="J15" s="543"/>
+      <c r="K15" s="543"/>
+      <c r="L15" s="525"/>
+      <c r="M15" s="524"/>
+      <c r="N15" s="525"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
@@ -24713,12 +25432,12 @@
       <c r="F16" s="460"/>
       <c r="G16" s="461"/>
       <c r="H16" s="462"/>
-      <c r="I16" s="507"/>
-      <c r="J16" s="573"/>
-      <c r="K16" s="573"/>
-      <c r="L16" s="508"/>
-      <c r="M16" s="507"/>
-      <c r="N16" s="508"/>
+      <c r="I16" s="524"/>
+      <c r="J16" s="543"/>
+      <c r="K16" s="543"/>
+      <c r="L16" s="525"/>
+      <c r="M16" s="524"/>
+      <c r="N16" s="525"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
@@ -24735,12 +25454,12 @@
       <c r="F17" s="460"/>
       <c r="G17" s="461"/>
       <c r="H17" s="462"/>
-      <c r="I17" s="507"/>
-      <c r="J17" s="573"/>
-      <c r="K17" s="573"/>
-      <c r="L17" s="508"/>
-      <c r="M17" s="507"/>
-      <c r="N17" s="508"/>
+      <c r="I17" s="524"/>
+      <c r="J17" s="543"/>
+      <c r="K17" s="543"/>
+      <c r="L17" s="525"/>
+      <c r="M17" s="524"/>
+      <c r="N17" s="525"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
@@ -24755,12 +25474,12 @@
       <c r="F18" s="463"/>
       <c r="G18" s="464"/>
       <c r="H18" s="465"/>
-      <c r="I18" s="509"/>
-      <c r="J18" s="574"/>
-      <c r="K18" s="574"/>
-      <c r="L18" s="510"/>
-      <c r="M18" s="509"/>
-      <c r="N18" s="510"/>
+      <c r="I18" s="526"/>
+      <c r="J18" s="544"/>
+      <c r="K18" s="544"/>
+      <c r="L18" s="527"/>
+      <c r="M18" s="526"/>
+      <c r="N18" s="527"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
@@ -24836,29 +25555,29 @@
       <c r="S21" s="9"/>
     </row>
     <row r="24" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B24" s="519" t="s">
+      <c r="B24" s="510" t="s">
         <v>570</v>
       </c>
-      <c r="C24" s="519"/>
-      <c r="D24" s="518"/>
-      <c r="E24" s="518"/>
-      <c r="F24" s="518"/>
-      <c r="G24" s="518"/>
-      <c r="H24" s="518"/>
-      <c r="I24" s="518"/>
-      <c r="J24" s="518"/>
-      <c r="K24" s="518"/>
-      <c r="M24" s="541" t="s">
+      <c r="C24" s="510"/>
+      <c r="D24" s="509"/>
+      <c r="E24" s="509"/>
+      <c r="F24" s="509"/>
+      <c r="G24" s="509"/>
+      <c r="H24" s="509"/>
+      <c r="I24" s="509"/>
+      <c r="J24" s="509"/>
+      <c r="K24" s="509"/>
+      <c r="M24" s="563" t="s">
         <v>179</v>
       </c>
-      <c r="N24" s="541"/>
-      <c r="O24" s="541"/>
+      <c r="N24" s="563"/>
+      <c r="O24" s="563"/>
     </row>
     <row r="25" spans="2:19" ht="15.75" thickBot="1">
-      <c r="B25" s="542" t="s">
+      <c r="B25" s="564" t="s">
         <v>913</v>
       </c>
-      <c r="C25" s="486"/>
+      <c r="C25" s="487"/>
       <c r="D25" s="435" t="s">
         <v>178</v>
       </c>
@@ -24880,13 +25599,13 @@
       </c>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="487"/>
-      <c r="C26" s="488"/>
-      <c r="D26" s="485" t="s">
+      <c r="B26" s="488"/>
+      <c r="C26" s="489"/>
+      <c r="D26" s="486" t="s">
         <v>906</v>
       </c>
-      <c r="E26" s="486"/>
-      <c r="F26" s="569" t="s">
+      <c r="E26" s="487"/>
+      <c r="F26" s="557" t="s">
         <v>906</v>
       </c>
       <c r="G26" s="435"/>
@@ -24910,22 +25629,22 @@
       </c>
     </row>
     <row r="27" spans="2:19">
-      <c r="B27" s="487"/>
-      <c r="C27" s="488"/>
-      <c r="D27" s="482" t="s">
+      <c r="B27" s="488"/>
+      <c r="C27" s="489"/>
+      <c r="D27" s="478" t="s">
         <v>911</v>
       </c>
-      <c r="E27" s="488"/>
-      <c r="F27" s="487" t="s">
+      <c r="E27" s="489"/>
+      <c r="F27" s="488" t="s">
         <v>907</v>
       </c>
-      <c r="G27" s="482"/>
-      <c r="H27" s="553"/>
-      <c r="I27" s="552" t="s">
+      <c r="G27" s="478"/>
+      <c r="H27" s="558"/>
+      <c r="I27" s="562" t="s">
         <v>911</v>
       </c>
-      <c r="J27" s="482"/>
-      <c r="K27" s="553"/>
+      <c r="J27" s="478"/>
+      <c r="K27" s="558"/>
       <c r="L27" s="5" t="s">
         <v>2</v>
       </c>
@@ -24940,22 +25659,22 @@
       </c>
     </row>
     <row r="28" spans="2:19">
-      <c r="B28" s="487"/>
-      <c r="C28" s="488"/>
-      <c r="D28" s="482" t="s">
+      <c r="B28" s="488"/>
+      <c r="C28" s="489"/>
+      <c r="D28" s="478" t="s">
         <v>908</v>
       </c>
-      <c r="E28" s="488"/>
-      <c r="F28" s="487" t="s">
+      <c r="E28" s="489"/>
+      <c r="F28" s="488" t="s">
         <v>908</v>
       </c>
-      <c r="G28" s="482"/>
-      <c r="H28" s="553"/>
-      <c r="I28" s="552" t="s">
+      <c r="G28" s="478"/>
+      <c r="H28" s="558"/>
+      <c r="I28" s="562" t="s">
         <v>908</v>
       </c>
-      <c r="J28" s="482"/>
-      <c r="K28" s="553"/>
+      <c r="J28" s="478"/>
+      <c r="K28" s="558"/>
       <c r="L28" s="5" t="s">
         <v>2</v>
       </c>
@@ -24964,22 +25683,22 @@
       <c r="O28" s="38"/>
     </row>
     <row r="29" spans="2:19">
-      <c r="B29" s="489"/>
-      <c r="C29" s="490"/>
-      <c r="D29" s="482" t="s">
+      <c r="B29" s="490"/>
+      <c r="C29" s="491"/>
+      <c r="D29" s="478" t="s">
         <v>909</v>
       </c>
-      <c r="E29" s="488"/>
-      <c r="F29" s="570" t="s">
+      <c r="E29" s="489"/>
+      <c r="F29" s="559" t="s">
         <v>909</v>
       </c>
-      <c r="G29" s="555"/>
-      <c r="H29" s="556"/>
-      <c r="I29" s="554" t="s">
+      <c r="G29" s="560"/>
+      <c r="H29" s="561"/>
+      <c r="I29" s="574" t="s">
         <v>909</v>
       </c>
-      <c r="J29" s="555"/>
-      <c r="K29" s="556"/>
+      <c r="J29" s="560"/>
+      <c r="K29" s="561"/>
       <c r="L29" s="24" t="s">
         <v>2</v>
       </c>
@@ -24992,20 +25711,20 @@
         <v>912</v>
       </c>
       <c r="C30" s="439"/>
-      <c r="D30" s="557" t="s">
+      <c r="D30" s="545" t="s">
         <v>571</v>
       </c>
-      <c r="E30" s="558"/>
-      <c r="F30" s="562" t="s">
+      <c r="E30" s="546"/>
+      <c r="F30" s="550" t="s">
         <v>572</v>
       </c>
-      <c r="G30" s="563"/>
-      <c r="H30" s="558"/>
-      <c r="I30" s="562" t="s">
+      <c r="G30" s="551"/>
+      <c r="H30" s="546"/>
+      <c r="I30" s="550" t="s">
         <v>573</v>
       </c>
-      <c r="J30" s="563"/>
-      <c r="K30" s="566"/>
+      <c r="J30" s="551"/>
+      <c r="K30" s="554"/>
       <c r="L30" s="5"/>
       <c r="M30" s="38"/>
       <c r="N30" s="38"/>
@@ -25014,14 +25733,14 @@
     <row r="31" spans="2:19">
       <c r="B31" s="420"/>
       <c r="C31" s="440"/>
-      <c r="D31" s="559"/>
-      <c r="E31" s="525"/>
-      <c r="F31" s="523"/>
-      <c r="G31" s="524"/>
-      <c r="H31" s="525"/>
-      <c r="I31" s="523"/>
-      <c r="J31" s="524"/>
-      <c r="K31" s="567"/>
+      <c r="D31" s="547"/>
+      <c r="E31" s="507"/>
+      <c r="F31" s="505"/>
+      <c r="G31" s="506"/>
+      <c r="H31" s="507"/>
+      <c r="I31" s="505"/>
+      <c r="J31" s="506"/>
+      <c r="K31" s="555"/>
       <c r="L31" s="5"/>
       <c r="M31" s="38"/>
       <c r="N31" s="38"/>
@@ -25030,107 +25749,107 @@
     <row r="32" spans="2:19">
       <c r="B32" s="420"/>
       <c r="C32" s="440"/>
-      <c r="D32" s="559"/>
-      <c r="E32" s="525"/>
-      <c r="F32" s="523"/>
-      <c r="G32" s="524"/>
-      <c r="H32" s="525"/>
-      <c r="I32" s="523"/>
-      <c r="J32" s="524"/>
-      <c r="K32" s="567"/>
+      <c r="D32" s="547"/>
+      <c r="E32" s="507"/>
+      <c r="F32" s="505"/>
+      <c r="G32" s="506"/>
+      <c r="H32" s="507"/>
+      <c r="I32" s="505"/>
+      <c r="J32" s="506"/>
+      <c r="K32" s="555"/>
       <c r="L32" s="5"/>
     </row>
     <row r="33" spans="2:14">
       <c r="B33" s="420"/>
       <c r="C33" s="440"/>
-      <c r="D33" s="560"/>
-      <c r="E33" s="561"/>
-      <c r="F33" s="564"/>
-      <c r="G33" s="565"/>
-      <c r="H33" s="561"/>
-      <c r="I33" s="564"/>
-      <c r="J33" s="565"/>
-      <c r="K33" s="568"/>
+      <c r="D33" s="548"/>
+      <c r="E33" s="549"/>
+      <c r="F33" s="552"/>
+      <c r="G33" s="553"/>
+      <c r="H33" s="549"/>
+      <c r="I33" s="552"/>
+      <c r="J33" s="553"/>
+      <c r="K33" s="556"/>
     </row>
     <row r="34" spans="2:14">
       <c r="B34" s="420"/>
       <c r="C34" s="422"/>
-      <c r="D34" s="543" t="s">
+      <c r="D34" s="565" t="s">
         <v>899</v>
       </c>
-      <c r="E34" s="544"/>
-      <c r="F34" s="543" t="s">
+      <c r="E34" s="566"/>
+      <c r="F34" s="565" t="s">
         <v>593</v>
       </c>
-      <c r="G34" s="549"/>
-      <c r="H34" s="544"/>
-      <c r="I34" s="543" t="s">
+      <c r="G34" s="571"/>
+      <c r="H34" s="566"/>
+      <c r="I34" s="565" t="s">
         <v>914</v>
       </c>
-      <c r="J34" s="549"/>
-      <c r="K34" s="544"/>
+      <c r="J34" s="571"/>
+      <c r="K34" s="566"/>
     </row>
     <row r="35" spans="2:14">
       <c r="B35" s="420"/>
       <c r="C35" s="422"/>
-      <c r="D35" s="545"/>
-      <c r="E35" s="546"/>
-      <c r="F35" s="545"/>
-      <c r="G35" s="550"/>
-      <c r="H35" s="546"/>
-      <c r="I35" s="545"/>
-      <c r="J35" s="550"/>
-      <c r="K35" s="546"/>
+      <c r="D35" s="567"/>
+      <c r="E35" s="568"/>
+      <c r="F35" s="567"/>
+      <c r="G35" s="572"/>
+      <c r="H35" s="568"/>
+      <c r="I35" s="567"/>
+      <c r="J35" s="572"/>
+      <c r="K35" s="568"/>
     </row>
     <row r="36" spans="2:14">
       <c r="B36" s="420"/>
       <c r="C36" s="422"/>
-      <c r="D36" s="545"/>
-      <c r="E36" s="546"/>
-      <c r="F36" s="545"/>
-      <c r="G36" s="550"/>
-      <c r="H36" s="546"/>
-      <c r="I36" s="545"/>
-      <c r="J36" s="550"/>
-      <c r="K36" s="546"/>
+      <c r="D36" s="567"/>
+      <c r="E36" s="568"/>
+      <c r="F36" s="567"/>
+      <c r="G36" s="572"/>
+      <c r="H36" s="568"/>
+      <c r="I36" s="567"/>
+      <c r="J36" s="572"/>
+      <c r="K36" s="568"/>
     </row>
     <row r="37" spans="2:14">
       <c r="B37" s="420"/>
       <c r="C37" s="422"/>
-      <c r="D37" s="545"/>
-      <c r="E37" s="546"/>
-      <c r="F37" s="545"/>
-      <c r="G37" s="550"/>
-      <c r="H37" s="546"/>
-      <c r="I37" s="545"/>
-      <c r="J37" s="550"/>
-      <c r="K37" s="546"/>
+      <c r="D37" s="567"/>
+      <c r="E37" s="568"/>
+      <c r="F37" s="567"/>
+      <c r="G37" s="572"/>
+      <c r="H37" s="568"/>
+      <c r="I37" s="567"/>
+      <c r="J37" s="572"/>
+      <c r="K37" s="568"/>
     </row>
     <row r="38" spans="2:14" ht="15.75" thickBot="1">
       <c r="B38" s="420"/>
       <c r="C38" s="422"/>
-      <c r="D38" s="547"/>
-      <c r="E38" s="548"/>
-      <c r="F38" s="547"/>
-      <c r="G38" s="551"/>
-      <c r="H38" s="548"/>
-      <c r="I38" s="547"/>
-      <c r="J38" s="551"/>
-      <c r="K38" s="548"/>
+      <c r="D38" s="569"/>
+      <c r="E38" s="570"/>
+      <c r="F38" s="569"/>
+      <c r="G38" s="573"/>
+      <c r="H38" s="570"/>
+      <c r="I38" s="569"/>
+      <c r="J38" s="573"/>
+      <c r="K38" s="570"/>
     </row>
     <row r="39" spans="2:14" ht="19.5" thickBot="1">
       <c r="B39" s="441"/>
       <c r="C39" s="443"/>
-      <c r="D39" s="527" t="s">
+      <c r="D39" s="498" t="s">
         <v>574</v>
       </c>
-      <c r="E39" s="528"/>
-      <c r="F39" s="528"/>
-      <c r="G39" s="528"/>
-      <c r="H39" s="528"/>
-      <c r="I39" s="528"/>
-      <c r="J39" s="528"/>
-      <c r="K39" s="529"/>
+      <c r="E39" s="499"/>
+      <c r="F39" s="499"/>
+      <c r="G39" s="499"/>
+      <c r="H39" s="499"/>
+      <c r="I39" s="499"/>
+      <c r="J39" s="499"/>
+      <c r="K39" s="500"/>
       <c r="L39" s="40" t="s">
         <v>575</v>
       </c>
@@ -25167,16 +25886,17 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="E4:E18"/>
-    <mergeCell ref="M5:N18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:L20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="F5:H18"/>
-    <mergeCell ref="I5:L18"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="B30:C39"/>
+    <mergeCell ref="B25:C29"/>
+    <mergeCell ref="D34:E38"/>
+    <mergeCell ref="F34:H38"/>
+    <mergeCell ref="I34:K38"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D41:E41"/>
     <mergeCell ref="F41:K41"/>
@@ -25193,17 +25913,16 @@
     <mergeCell ref="F29:H29"/>
     <mergeCell ref="I26:K26"/>
     <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="B30:C39"/>
-    <mergeCell ref="B25:C29"/>
-    <mergeCell ref="D34:E38"/>
-    <mergeCell ref="F34:H38"/>
-    <mergeCell ref="I34:K38"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="F20:L20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="F5:H18"/>
+    <mergeCell ref="I5:L18"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="E4:E18"/>
+    <mergeCell ref="M5:N18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="R7" r:id="rId1"/>

</xml_diff>